<commit_message>
fix: adjust xpath expressions
</commit_message>
<xml_diff>
--- a/dedup/dedup_Toko_Oleh_Oleh.xlsx
+++ b/dedup/dedup_Toko_Oleh_Oleh.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K134"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,35 +456,30 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>reviews_count</t>
+          <t>reviews_average</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>reviews_average</t>
+          <t>latitude</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>latitude</t>
+          <t>longitude</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>longitude</t>
+          <t>is_permanently_closed</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>is_permanently_closed</t>
+          <t>gmaps_link</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>gmaps_link</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>latest_review_date</t>
         </is>
@@ -500,22 +495,21 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>-7.897066</v>
+      </c>
       <c r="G2" t="n">
-        <v>-7.897066</v>
-      </c>
-      <c r="H2" t="n">
         <v>110.323286</v>
       </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Geplak+Mbok+Tumpuk/@-7.8970663,110.251188,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7aff6500000001:0xf1057df9d7154d21!8m2!3d-7.8970663!4d110.3232858!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEEZGVsaeABAA!16s%2Fg%2F1pzs0p3w4?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -534,25 +528,24 @@
           <t>(0274) 367364</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F3" t="n">
-        <v>4.3</v>
+        <v>-7.883165</v>
       </c>
       <c r="G3" t="n">
-        <v>-7.883165</v>
-      </c>
-      <c r="H3" t="n">
         <v>110.332046</v>
       </c>
-      <c r="I3" t="b">
-        <v>0</v>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Kurnia+Bantul/@-7.8970663,110.251188,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55ff6d916af5:0x181c9758ce86da5e!8m2!3d-7.8831655!4d110.3320459!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgETc2Nob29sX3N1cHBseV9zdG9yZeABAA!16s%2Fg%2F11b6mhtdn1?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J3" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Kurnia+Bantul/@-7.8970663,110.251188,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55ff6d916af5:0x181c9758ce86da5e!8m2!3d-7.8831655!4d110.3320459!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgETc2Nob29sX3N1cHBseV9zdG9yZeABAA!16s%2Fg%2F11b6mhtdn1?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -571,25 +564,24 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>3.9</v>
+      </c>
       <c r="F4" t="n">
-        <v>3.9</v>
+        <v>-7.938418</v>
       </c>
       <c r="G4" t="n">
-        <v>-7.938418</v>
-      </c>
-      <c r="H4" t="n">
         <v>110.337473</v>
       </c>
-      <c r="I4" t="b">
-        <v>0</v>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+oleh+oleh+Bu+vera+-+Paris/@-7.8970663,110.251188,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5566da2d563b:0x9775a498eb77163a!8m2!3d-7.9384177!4d110.3374733!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVTjRhbVpoV0doUlJSQULgAQD6AQQIABA8!16s%2Fg%2F11g8yk100g?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J4" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+oleh+oleh+Bu+vera+-+Paris/@-7.8970663,110.251188,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5566da2d563b:0x9775a498eb77163a!8m2!3d-7.9384177!4d110.3374733!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVTjRhbVpoV0doUlJSQULgAQD6AQQIABA8!16s%2Fg%2F11g8yk100g?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
         <is>
           <t>2 hari lalu</t>
         </is>
@@ -608,25 +600,24 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>3.9</v>
+      </c>
       <c r="F5" t="n">
-        <v>3.9</v>
+        <v>-7.926734</v>
       </c>
       <c r="G5" t="n">
-        <v>-7.926734</v>
-      </c>
-      <c r="H5" t="n">
         <v>110.281638</v>
       </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Oleh+Oleh+Bantul+Yogyakarta/@-7.9267345,110.20954,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7afe54e0eab69f:0xa6c1185d3823fda2!8m2!3d-7.9267345!4d110.2816378!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEPc2hvcHBpbmdfY2VudGVymgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVVJ1ZWpjeWJuUjNSUkFC4AEA-gEECAAQLQ!16s%2Fg%2F11gcqwvl4j?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -645,25 +636,24 @@
           <t>0877-3824-2244</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F6" t="n">
-        <v>4.5</v>
+        <v>-7.898807</v>
       </c>
       <c r="G6" t="n">
-        <v>-7.898807</v>
-      </c>
-      <c r="H6" t="n">
         <v>110.372953</v>
       </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr">
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Spesialis+Brownies+Panggang+dan+Roti+Hantaran+RAHAPI/@-7.8988073,110.3008551,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55672403e37f:0x2258003aee93ecfc!8m2!3d-7.8988073!4d110.3729529!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEJY2FrZV9zaG9w4AEA!16s%2Fg%2F11jp74hjhw?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -682,25 +672,24 @@
           <t>0856-4376-9657</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F7" t="n">
-        <v>4.9</v>
+        <v>-7.793935</v>
       </c>
       <c r="G7" t="n">
-        <v>-7.793935</v>
-      </c>
-      <c r="H7" t="n">
         <v>110.367778</v>
       </c>
-      <c r="I7" t="b">
-        <v>0</v>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Oleh-oleh+Khas+Jogja+BU+TINI/@-7.7939353,110.2956801,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a582840a0f525:0x9109beec43928361!8m2!3d-7.7939353!4d110.3677779!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F1hm5669kf?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J7" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Oleh-oleh+Khas+Jogja+BU+TINI/@-7.7939353,110.2956801,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a582840a0f525:0x9109beec43928361!8m2!3d-7.7939353!4d110.3677779!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F1hm5669kf?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
         <is>
           <t>seminggu lalu</t>
         </is>
@@ -719,25 +708,24 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>3.4</v>
+      </c>
       <c r="F8" t="n">
-        <v>3.4</v>
+        <v>-7.82605</v>
       </c>
       <c r="G8" t="n">
-        <v>-7.82605</v>
-      </c>
-      <c r="H8" t="n">
         <v>110.354337</v>
       </c>
-      <c r="I8" t="b">
-        <v>0</v>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/NICESO+BANTUL/@-7.7939353,110.2956801,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5744b81b8e01:0xafec742da50f2963!8m2!3d-7.8260503!4d110.3543373!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgERY29udmVuaWVuY2Vfc3RvcmWaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVUkNOSFkyY2s1UkVBReABAPoBBAgAEEM!16s%2Fg%2F11tj2yml97?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J8" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/NICESO+BANTUL/@-7.7939353,110.2956801,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5744b81b8e01:0xafec742da50f2963!8m2!3d-7.8260503!4d110.3543373!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgERY29udmVuaWVuY2Vfc3RvcmWaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVUkNOSFkyY2s1UkVBReABAPoBBAgAEEM!16s%2Fg%2F11tj2yml97?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
         <is>
           <t>3 minggu lalu</t>
         </is>
@@ -760,25 +748,24 @@
           <t>0823-3845-1712</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F9" t="n">
-        <v>4.8</v>
+        <v>-7.814294</v>
       </c>
       <c r="G9" t="n">
-        <v>-7.814294</v>
-      </c>
-      <c r="H9" t="n">
         <v>110.3561</v>
       </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" t="inlineStr">
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Pusat+Oleh+Oleh+Ob/@-7.7939353,110.2956801,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5794dfb4efa9:0x3a0b31d7a23c6c1!8m2!3d-7.8142945!4d110.3561001!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWySAQpmb29kX3N0b3Jl4AEA!16s%2Fg%2F11bbx28q0c?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -797,25 +784,24 @@
           <t>(0274) 6536960</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>3.9</v>
+      </c>
       <c r="F10" t="n">
-        <v>3.9</v>
+        <v>-7.885327</v>
       </c>
       <c r="G10" t="n">
-        <v>-7.885327</v>
-      </c>
-      <c r="H10" t="n">
         <v>110.329565</v>
       </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+dan+Camilan+Bu+Nurul/@-7.8853267,110.2574671,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7aff55e4940f4f:0xac4ad12d6e82a8de!8m2!3d-7.8853267!4d110.3295649!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEKZm9vZF9zdG9yZZoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VSVWVWOW1XSEYzUlJBQuABAPoBBAgAEDc!16s%2Fg%2F11b6nnb7k9?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -830,25 +816,24 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F11" t="n">
-        <v>4.6</v>
+        <v>-7.908816</v>
       </c>
       <c r="G11" t="n">
-        <v>-7.908816</v>
-      </c>
-      <c r="H11" t="n">
         <v>110.351938</v>
       </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" t="inlineStr">
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Pusat+Oleh2+Lancar/@-7.8853267,110.2574671,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55979f76df43:0x9b8031d4bb35e534!8m2!3d-7.9088161!4d110.3519382!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgELc3VwZXJtYXJrZXTgAQA!16s%2Fg%2F11fz9h_rnr?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -871,25 +856,24 @@
           <t>0821-4038-4686</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F12" t="n">
-        <v>4.6</v>
+        <v>-7.79651</v>
       </c>
       <c r="G12" t="n">
-        <v>-7.79651</v>
-      </c>
-      <c r="H12" t="n">
         <v>110.343207</v>
       </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="inlineStr">
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Art+elektronik/@-7.7965097,110.2711091,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a59ac6602d0ef:0xe62fae3bde670fa7!8m2!3d-7.7965097!4d110.3432069!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgERZWxlY3Ryb25pY3Nfc3RvcmXgAQA!16s%2Fg%2F11k20dz4xx?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -904,25 +888,24 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F13" t="n">
-        <v>4.5</v>
+        <v>-7.805191</v>
       </c>
       <c r="G13" t="n">
-        <v>-7.805191</v>
-      </c>
-      <c r="H13" t="n">
         <v>110.360353</v>
       </c>
-      <c r="I13" t="b">
-        <v>0</v>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh+-+Oleh+Terlengkap/@-7.7965097,110.2711091,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a578dde7f1329:0x76945642e488661d!8m2!3d-7.805191!4d110.3603533!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F11jk6kmz5v?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J13" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh+-+Oleh+Terlengkap/@-7.7965097,110.2711091,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a578dde7f1329:0x76945642e488661d!8m2!3d-7.805191!4d110.3603533!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F11jk6kmz5v?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
         <is>
           <t>seminggu lalu</t>
         </is>
@@ -945,25 +928,24 @@
           <t>(0274) 580586</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F14" t="n">
-        <v>4.4</v>
+        <v>-7.800828</v>
       </c>
       <c r="G14" t="n">
-        <v>-7.800828</v>
-      </c>
-      <c r="H14" t="n">
         <v>110.348561</v>
       </c>
-      <c r="I14" t="b">
-        <v>0</v>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Intisari+Martadinata/@-7.7965097,110.2711091,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57f6a1ce887d:0x2104e7472c3cd782!8m2!3d-7.8008278!4d110.3485612!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgETYmFraW5nX3N1cHBseV9zdG9yZeABAA!16s%2Fg%2F11b6dylgbx?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J14" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Intisari+Martadinata/@-7.7965097,110.2711091,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57f6a1ce887d:0x2104e7472c3cd782!8m2!3d-7.8008278!4d110.3485612!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgETYmFraW5nX3N1cHBseV9zdG9yZeABAA!16s%2Fg%2F11b6dylgbx?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
         <is>
           <t>6 hari lalu</t>
         </is>
@@ -986,25 +968,24 @@
           <t>0882-0053-65176</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
       <c r="F15" t="n">
-        <v>5</v>
+        <v>-7.89192</v>
       </c>
       <c r="G15" t="n">
-        <v>-7.89192</v>
-      </c>
-      <c r="H15" t="n">
         <v>110.352356</v>
       </c>
-      <c r="I15" t="b">
-        <v>0</v>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/JIMSHONEY+BANTUL+STORE+OFFICIAL+(Jimshoney+jogja+store+official)/@-7.8919196,110.2802579,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55f531c71601:0x1e7beeb6abfa65b!8m2!3d-7.8919196!4d110.3523557!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEIYmFnX3Nob3DgAQA!16s%2Fg%2F11sf0dhz1h?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J15" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/JIMSHONEY+BANTUL+STORE+OFFICIAL+(Jimshoney+jogja+store+official)/@-7.8919196,110.2802579,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55f531c71601:0x1e7beeb6abfa65b!8m2!3d-7.8919196!4d110.3523557!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEIYmFnX3Nob3DgAQA!16s%2Fg%2F11sf0dhz1h?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -1031,25 +1012,24 @@
           <t>0877-4233-9130</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F16" t="n">
-        <v>4.5</v>
+        <v>-7.804458</v>
       </c>
       <c r="G16" t="n">
-        <v>-7.804458</v>
-      </c>
-      <c r="H16" t="n">
         <v>110.342983</v>
       </c>
-      <c r="I16" t="b">
-        <v>0</v>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Danar+Koper+Bantul/@-7.8044577,110.2708854,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57db6b28ebb1:0x10f582c4ec5d43a3!8m2!3d-7.8044577!4d110.3429832!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgENbHVnZ2FnZV9zdG9yZeABAA!16s%2Fg%2F11gh9pq4cz?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J16" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Danar+Koper+Bantul/@-7.8044577,110.2708854,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57db6b28ebb1:0x10f582c4ec5d43a3!8m2!3d-7.8044577!4d110.3429832!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgENbHVnZ2FnZV9zdG9yZeABAA!16s%2Fg%2F11gh9pq4cz?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -1072,25 +1052,24 @@
           <t>0851-0245-0808</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>3.7</v>
+      </c>
       <c r="F17" t="n">
-        <v>3.7</v>
+        <v>-7.893598</v>
       </c>
       <c r="G17" t="n">
-        <v>-7.893598</v>
-      </c>
-      <c r="H17" t="n">
         <v>110.341237</v>
       </c>
-      <c r="I17" t="b">
-        <v>0</v>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+%26+Camilan+%22Lancar%22/@-7.8935985,110.2691391,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55f1bf68e45f:0xb05084f8c15babd5!8m2!3d-7.8935985!4d110.3412369!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgERaGVhbHRoX2Zvb2Rfc3RvcmXgAQA!16s%2Fg%2F11b6jg_z62?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J17" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+%26+Camilan+%22Lancar%22/@-7.8935985,110.2691391,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55f1bf68e45f:0xb05084f8c15babd5!8m2!3d-7.8935985!4d110.3412369!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgERaGVhbHRoX2Zvb2Rfc3RvcmXgAQA!16s%2Fg%2F11b6jg_z62?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
         <is>
           <t>2 tahun lalu</t>
         </is>
@@ -1117,25 +1096,24 @@
           <t>0831-3875-1329</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F18" t="n">
-        <v>4.6</v>
+        <v>-7.814432</v>
       </c>
       <c r="G18" t="n">
-        <v>-7.814432</v>
-      </c>
-      <c r="H18" t="n">
         <v>110.355829</v>
       </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" t="inlineStr">
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/JOSS+GANDOS+PUSAT+YOGYAKARTA/@-7.8144322,110.2837309,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5794d8b0dda3:0x840ad238dbe47a63!8m2!3d-7.8144322!4d110.3558287!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEOY29tcHV0ZXJfc3RvcmXgAQA!16s%2Fg%2F11bztjbbdc?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1155,22 +1133,21 @@
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>-7.830055</v>
+      </c>
       <c r="G19" t="n">
-        <v>-7.830055</v>
-      </c>
-      <c r="H19" t="n">
         <v>110.367463</v>
       </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" t="inlineStr">
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Toko+Diantama+-+Ruko+Perwita+Regency%EA%A7%8B%EA%A6%A0%EA%A6%BA%EA%A6%B4%EA%A6%8F%EA%A6%BA%EA%A6%B4%EA%A6%A3%EA%A6%B6%EA%A6%AA%EA%A6%A4%EA%A7%80%EA%A6%A0%EA%A6%A9%EA%A6%AB%EA%A6%B8%EA%A6%8F%EA%A6%BA%EA%A6%B4%EA%A6%A5%EA%A6%BC%EA%A6%82%EA%A6%AE%EA%A6%B6%EA%A6%A0%EA%A6%89%EA%A6%92%EA%A6%BC%EA%A6%9A%EA%A7%80%EA%A6%95%EA%A7%80%EA%A6%AA%EA%A7%80/@-7.8144322,110.2837309,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57ae3032b3af:0x595bf253c7c2e7a7!8m2!3d-7.8300549!4d110.3674631!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgELY3JhZnRfc3RvcmXgAQA!16s%2Fg%2F1hm3kd7kf?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1189,25 +1166,24 @@
           <t>0818-0421-3977</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>4.2</v>
+      </c>
       <c r="F20" t="n">
-        <v>4.2</v>
+        <v>-7.916758</v>
       </c>
       <c r="G20" t="n">
-        <v>-7.916758</v>
-      </c>
-      <c r="H20" t="n">
         <v>110.38174</v>
       </c>
-      <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" t="inlineStr">
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Pasar+Imogiri+Bantul/@-7.9167581,110.3096425,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5455081ed15b:0xb77942b9cbe913dc!8m2!3d-7.9167581!4d110.3817403!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEOcHJvZHVjZV9tYXJrZXTgAQA!16s%2Fg%2F11cjpb0yt8?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1226,25 +1202,24 @@
           <t>0878-3832-0769</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="n">
+        <v>5</v>
+      </c>
       <c r="F21" t="n">
-        <v>5</v>
+        <v>-7.886084</v>
       </c>
       <c r="G21" t="n">
-        <v>-7.886084</v>
-      </c>
-      <c r="H21" t="n">
         <v>110.330328</v>
       </c>
-      <c r="I21" t="b">
-        <v>0</v>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+oleh-oleh+Laris+Baru+Pak+Wintolo/@-7.8860841,110.2582306,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7affb44b0c963d:0xf10202201c20b53!8m2!3d-7.8860841!4d110.3303284!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEPc2hvcHBpbmdfY2VudGVymgEjQ2haRFNVaE5NRzluUzBWSlEwRm5TVU5IYkVwTWNGTjNFQUXgAQD6AQQIABAc!16s%2Fg%2F11p6pbpv50?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J21" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+oleh-oleh+Laris+Baru+Pak+Wintolo/@-7.8860841,110.2582306,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7affb44b0c963d:0xf10202201c20b53!8m2!3d-7.8860841!4d110.3303284!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEPc2hvcHBpbmdfY2VudGVymgEjQ2haRFNVaE5NRzluUzBWSlEwRm5TVU5IYkVwTWNGTjNFQUXgAQD6AQQIABAc!16s%2Fg%2F11p6pbpv50?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
         <is>
           <t>3 tahun lalu</t>
         </is>
@@ -1267,25 +1242,24 @@
           <t>(0274) 388496</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F22" t="n">
-        <v>4.5</v>
+        <v>-7.824719</v>
       </c>
       <c r="G22" t="n">
-        <v>-7.824719</v>
-      </c>
-      <c r="H22" t="n">
         <v>110.373024</v>
       </c>
-      <c r="I22" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" t="inlineStr">
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Dapur+Roti+Bu+Haryati(%EA%A7%8B%EA%A6%A3%EA%A6%A5%EA%A6%B8%EA%A6%82%EA%A6%AB%EA%A6%BA%EA%A6%B4%EA%A6%A0%EA%A6%B6%EA%A6%A7%EA%A6%B8%EA%A6%B2%EA%A6%82%EA%A6%AA%EA%A6%A0%EA%A6%B6)/@-7.8247189,110.3009261,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57a5d7e6e633:0xd4f24ab31d55279!8m2!3d-7.8247189!4d110.3730239!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEGYmFrZXJ54AEA!16s%2Fg%2F11bzywjh0v?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1304,25 +1278,24 @@
           <t>0852-9345-4133</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F23" t="n">
-        <v>4.8</v>
+        <v>-7.935834</v>
       </c>
       <c r="G23" t="n">
-        <v>-7.935834</v>
-      </c>
-      <c r="H23" t="n">
         <v>110.369583</v>
       </c>
-      <c r="I23" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" t="inlineStr">
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/BAKPIA+PATHOK+DINDUN/@-7.9358345,110.2974853,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55199d9b6a93:0xbf90795f60dc2095!8m2!3d-7.9358345!4d110.3695831!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEJY2FrZV9zaG9w4AEA!16s%2Fg%2F11gb409m98?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1341,25 +1314,24 @@
           <t>0852-9345-4133</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F24" t="n">
-        <v>4.8</v>
+        <v>-7.891692</v>
       </c>
       <c r="G24" t="n">
-        <v>-7.891692</v>
-      </c>
-      <c r="H24" t="n">
         <v>110.327859</v>
       </c>
-      <c r="I24" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" t="inlineStr">
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Mulia+Swalayan+%26+Toserba+Bantul/@-7.8916917,110.2557613,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7aff59cafcd819:0xb0495038615e495e!8m2!3d-7.8916917!4d110.3278591!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEQZGVwYXJ0bWVudF9zdG9yZeABAA!16s%2Fg%2F11b7lpdxk0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1382,25 +1354,24 @@
           <t>0817-9438-740</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>4.7</v>
+      </c>
       <c r="F25" t="n">
-        <v>4.7</v>
+        <v>-7.79497</v>
       </c>
       <c r="G25" t="n">
-        <v>-7.79497</v>
-      </c>
-      <c r="H25" t="n">
         <v>110.365348</v>
       </c>
-      <c r="I25" t="b">
-        <v>0</v>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Jogja+Pasaraya/@-7.7949698,110.2932502,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a59779366cb35:0x3aafac9b4832206c!8m2!3d-7.7949698!4d110.365348!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F11kgr0n7sw?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J25" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Jogja+Pasaraya/@-7.7949698,110.2932502,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a59779366cb35:0x3aafac9b4832206c!8m2!3d-7.7949698!4d110.365348!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F11kgr0n7sw?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
         <is>
           <t>seminggu lalu</t>
         </is>
@@ -1423,25 +1394,24 @@
           <t>0822-9873-9584</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="n">
+        <v>4.7</v>
+      </c>
       <c r="F26" t="n">
-        <v>4.7</v>
+        <v>-7.814968</v>
       </c>
       <c r="G26" t="n">
-        <v>-7.814968</v>
-      </c>
-      <c r="H26" t="n">
         <v>110.356179</v>
       </c>
-      <c r="I26" t="b">
-        <v>0</v>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Masrifah+Bakery+%26+Cake/@-7.7949698,110.2932502,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a579522fef471:0x1292eaee86ecad10!8m2!3d-7.8149682!4d110.3561785!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEGYmFrZXJ54AEA!16s%2Fg%2F11bbx0c_f5?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J26" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Masrifah+Bakery+%26+Cake/@-7.7949698,110.2932502,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a579522fef471:0x1292eaee86ecad10!8m2!3d-7.8149682!4d110.3561785!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEGYmFrZXJ54AEA!16s%2Fg%2F11bbx0c_f5?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
         <is>
           <t>5 bulan lalu</t>
         </is>
@@ -1464,25 +1434,24 @@
           <t>0813-2746-1162</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="n">
+        <v>5</v>
+      </c>
       <c r="F27" t="n">
-        <v>5</v>
+        <v>-7.828013</v>
       </c>
       <c r="G27" t="n">
-        <v>-7.828013</v>
-      </c>
-      <c r="H27" t="n">
         <v>110.367328</v>
       </c>
-      <c r="I27" t="b">
-        <v>0</v>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Optik+B+Riski+Bantul/@-7.7949698,110.2932502,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57ee5bf1cab3:0x9cec53a03f639e2b!8m2!3d-7.8280128!4d110.3673283!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEIb3B0aWNpYW7gAQA!16s%2Fg%2F11t5n5rx6m?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J27" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Optik+B+Riski+Bantul/@-7.7949698,110.2932502,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57ee5bf1cab3:0x9cec53a03f639e2b!8m2!3d-7.8280128!4d110.3673283!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEIb3B0aWNpYW7gAQA!16s%2Fg%2F11t5n5rx6m?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
         <is>
           <t>21 jam lalu</t>
         </is>
@@ -1505,25 +1474,24 @@
           <t>0858-6630-0241</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F28" t="n">
-        <v>4.9</v>
+        <v>-7.781288</v>
       </c>
       <c r="G28" t="n">
-        <v>-7.781288</v>
-      </c>
-      <c r="H28" t="n">
         <v>110.350374</v>
       </c>
-      <c r="I28" t="b">
-        <v>0</v>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Erafone+Godean+Bantul/@-7.7949698,110.2932502,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a59b3af5e6853:0xa8b89f2f65bf1f58!8m2!3d-7.7812877!4d110.3503741!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgERZWxlY3Ryb25pY3Nfc3RvcmXgAQA!16s%2Fg%2F11trhzr_hc?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J28" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Erafone+Godean+Bantul/@-7.7949698,110.2932502,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a59b3af5e6853:0xa8b89f2f65bf1f58!8m2!3d-7.7812877!4d110.3503741!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgERZWxlY3Ryb25pY3Nfc3RvcmXgAQA!16s%2Fg%2F11trhzr_hc?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -1546,25 +1514,24 @@
           <t>0818-0272-0003</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="n">
+        <v>4.2</v>
+      </c>
       <c r="F29" t="n">
-        <v>4.2</v>
+        <v>-7.915509</v>
       </c>
       <c r="G29" t="n">
-        <v>-7.915509</v>
-      </c>
-      <c r="H29" t="n">
         <v>110.351644</v>
       </c>
-      <c r="I29" t="b">
-        <v>0</v>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh+Oleh+Geplak+Peyek+Tumpuk+Bantul/@-7.9155091,110.2795461,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55495935cd4b:0x2340deb5d30999a6!8m2!3d-7.9155091!4d110.3516439!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEZZm9vZF9tYW51ZmFjdHVyaW5nX3N1cHBseZoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VReWRDMVFPRlZuRUFF4AEA-gEFCKABED8!16s%2Fg%2F1pzrfpsy9?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J29" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh+Oleh+Geplak+Peyek+Tumpuk+Bantul/@-7.9155091,110.2795461,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55495935cd4b:0x2340deb5d30999a6!8m2!3d-7.9155091!4d110.3516439!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEZZm9vZF9tYW51ZmFjdHVyaW5nX3N1cHBseZoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VReWRDMVFPRlZuRUFF4AEA-gEFCKABED8!16s%2Fg%2F1pzrfpsy9?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
         <is>
           <t>seminggu lalu</t>
         </is>
@@ -1587,25 +1554,24 @@
           <t>0818-0272-0003</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="n">
+        <v>4.2</v>
+      </c>
       <c r="F30" t="n">
-        <v>4.2</v>
+        <v>-7.816542</v>
       </c>
       <c r="G30" t="n">
-        <v>-7.816542</v>
-      </c>
-      <c r="H30" t="n">
         <v>110.32832</v>
       </c>
-      <c r="I30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J30" t="inlineStr">
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/SOCKISGOOD+BANTUL+(toko+kaos+kaki)/@-7.8165418,110.2562225,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7af96aa6a92867:0x97bf11eadb2bf183!8m2!3d-7.8165418!4d110.3283203!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F11llnv33zy?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1624,25 +1590,24 @@
           <t>0888-6534-403</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F31" t="n">
-        <v>4.9</v>
+        <v>-7.909234</v>
       </c>
       <c r="G31" t="n">
-        <v>-7.909234</v>
-      </c>
-      <c r="H31" t="n">
         <v>110.382924</v>
       </c>
-      <c r="I31" t="b">
-        <v>0</v>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Buket+Bantul+Jogja+(Bykay+Bouquet)/@-7.9092336,110.3108259,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55d0e5bf5af5:0x951f03079bbf2563!8m2!3d-7.9092336!4d110.3829237!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEHZmxvcmlzdOABAA!16s%2Fg%2F11tf56l8lc?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J31" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Buket+Bantul+Jogja+(Bykay+Bouquet)/@-7.9092336,110.3108259,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55d0e5bf5af5:0x951f03079bbf2563!8m2!3d-7.9092336!4d110.3829237!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEHZmxvcmlzdOABAA!16s%2Fg%2F11tf56l8lc?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -1665,25 +1630,24 @@
           <t>0888-0295-5748</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="n">
+        <v>5</v>
+      </c>
       <c r="F32" t="n">
-        <v>5</v>
+        <v>-7.815059</v>
       </c>
       <c r="G32" t="n">
-        <v>-7.815059</v>
-      </c>
-      <c r="H32" t="n">
         <v>110.355742</v>
       </c>
-      <c r="I32" t="b">
-        <v>0</v>
-      </c>
-      <c r="J32" t="inlineStr">
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Central+Bearings/@-7.8150588,110.2836445,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5795249049f9:0xb3513d8b9931274e!8m2!3d-7.8150588!4d110.3557423!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F1pzwfj53j?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1706,25 +1670,24 @@
           <t>0811-1111-298</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F33" t="n">
-        <v>4.5</v>
+        <v>-7.919997</v>
       </c>
       <c r="G33" t="n">
-        <v>-7.919997</v>
-      </c>
-      <c r="H33" t="n">
         <v>110.379082</v>
       </c>
-      <c r="I33" t="b">
-        <v>0</v>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bakpia+Imogiri+517/@-7.9199974,110.3069843,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a54ffe6764971:0x18663d87bbaed109!8m2!3d-7.9199974!4d110.3790821!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F11cjhs8y1m?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J33" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Bakpia+Imogiri+517/@-7.9199974,110.3069843,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a54ffe6764971:0x18663d87bbaed109!8m2!3d-7.9199974!4d110.3790821!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F11cjhs8y1m?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -1747,25 +1710,24 @@
           <t>0821-3454-2242</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F34" t="n">
-        <v>4.9</v>
+        <v>-7.913549</v>
       </c>
       <c r="G34" t="n">
-        <v>-7.913549</v>
-      </c>
-      <c r="H34" t="n">
         <v>110.370632</v>
       </c>
-      <c r="I34" t="b">
-        <v>0</v>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Bangunan+Jaya+Abadi+Bantul/@-7.9199974,110.3069843,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5517516e9c2d:0x1a3311465dc86739!8m2!3d-7.9135486!4d110.3706324!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEYYnVpbGRpbmdfbWF0ZXJpYWxzX3N0b3Jl4AEA!16s%2Fg%2F11btxcwk0b?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J34" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Bangunan+Jaya+Abadi+Bantul/@-7.9199974,110.3069843,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5517516e9c2d:0x1a3311465dc86739!8m2!3d-7.9135486!4d110.3706324!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEYYnVpbGRpbmdfbWF0ZXJpYWxzX3N0b3Jl4AEA!16s%2Fg%2F11btxcwk0b?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
         <is>
           <t>2 tahun lalu</t>
         </is>
@@ -1792,25 +1754,24 @@
           <t>0813-9365-4890</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F35" t="n">
-        <v>4.9</v>
+        <v>-7.826471</v>
       </c>
       <c r="G35" t="n">
-        <v>-7.826471</v>
-      </c>
-      <c r="H35" t="n">
         <v>110.37447</v>
       </c>
-      <c r="I35" t="b">
-        <v>0</v>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Kado+Wisudaku/@-7.8264711,110.3023721,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57a89deb0827:0x975169057a6c00a6!8m2!3d-7.8264711!4d110.3744699!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEJZ2lmdF9zaG9w4AEA!16s%2Fg%2F11b7hfr2cl?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J35" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Kado+Wisudaku/@-7.8264711,110.3023721,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57a89deb0827:0x975169057a6c00a6!8m2!3d-7.8264711!4d110.3744699!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEJZ2lmdF9zaG9w4AEA!16s%2Fg%2F11b7hfr2cl?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -1837,25 +1798,24 @@
           <t>0813-9365-4890</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F36" t="n">
-        <v>4.9</v>
+        <v>-7.81677</v>
       </c>
       <c r="G36" t="n">
-        <v>-7.81677</v>
-      </c>
-      <c r="H36" t="n">
         <v>110.35601</v>
       </c>
-      <c r="I36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J36" t="inlineStr">
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Momoyo+ice+cream%26fruit+tea+bantul/@-7.8264711,110.3023721,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5704c791b465:0xddb4a2b32e0df6e8!8m2!3d-7.8167705!4d110.3560095!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEOaWNlX2NyZWFtX3Nob3DgAQA!16s%2Fg%2F11l5lthzkt?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1874,25 +1834,24 @@
           <t>0895-4185-7686</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
+      <c r="E37" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F37" t="n">
-        <v>4.4</v>
+        <v>-7.91216</v>
       </c>
       <c r="G37" t="n">
-        <v>-7.91216</v>
-      </c>
-      <c r="H37" t="n">
         <v>110.38252</v>
       </c>
-      <c r="I37" t="b">
-        <v>0</v>
-      </c>
-      <c r="J37" t="inlineStr">
+      <c r="H37" t="b">
+        <v>0</v>
+      </c>
+      <c r="I37" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Viend's+Cake+%26+Tart+%EA%A6%AE%EA%A6%B3%EA%A6%B6%EA%A6%AA%EA%A6%BA%EA%A6%A4%EA%A7%80%EA%A6%9D%EA%A7%80'%EA%A6%B1%EA%A7%80%EA%A6%95%EA%A6%8F%EA%A6%BA%26%EA%A6%A0%EA%A6%82%EA%A6%A0%EA%A7%80/@-7.9121604,110.3104226,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5453bc40b4a5:0xf0534c9126484338!8m2!3d-7.9121604!4d110.3825204!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEGYmFrZXJ54AEA!16s%2Fg%2F11fmdlxn8q?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1915,25 +1874,24 @@
           <t>0857-2928-7188</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="n">
+        <v>5</v>
+      </c>
       <c r="F38" t="n">
-        <v>5</v>
+        <v>-7.941581</v>
       </c>
       <c r="G38" t="n">
-        <v>-7.941581</v>
-      </c>
-      <c r="H38" t="n">
         <v>110.351359</v>
       </c>
-      <c r="I38" t="b">
-        <v>0</v>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Monela+Handmade+(+toko+buket+bantul+)/@-7.9121604,110.3104226,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5541d18aa59b:0x92ea3405f763b887!8m2!3d-7.941581!4d110.351359!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEJZ2lmdF9zaG9w4AEA!16s%2Fg%2F11f0xrhnpn?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J38" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Monela+Handmade+(+toko+buket+bantul+)/@-7.9121604,110.3104226,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5541d18aa59b:0x92ea3405f763b887!8m2!3d-7.941581!4d110.351359!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEJZ2lmdF9zaG9w4AEA!16s%2Fg%2F11f0xrhnpn?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K38" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -1960,25 +1918,24 @@
           <t>0812-2886-5711</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
+      <c r="E39" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F39" t="n">
-        <v>4.8</v>
+        <v>-7.819914</v>
       </c>
       <c r="G39" t="n">
-        <v>-7.819914</v>
-      </c>
-      <c r="H39" t="n">
         <v>110.354443</v>
       </c>
-      <c r="I39" t="b">
-        <v>0</v>
-      </c>
-      <c r="J39" t="inlineStr">
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Ricie/@-7.8199142,110.2823455,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57632cd24919:0xd3d2910b74f23ed0!8m2!3d-7.8199142!4d110.3544433!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFZGluZXLgAQA!16s%2Fg%2F11h227tpy_?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1997,25 +1954,24 @@
           <t>0856-4383-7538</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="n">
+        <v>5</v>
+      </c>
       <c r="F40" t="n">
-        <v>5</v>
+        <v>-7.829851</v>
       </c>
       <c r="G40" t="n">
-        <v>-7.829851</v>
-      </c>
-      <c r="H40" t="n">
         <v>110.353797</v>
       </c>
-      <c r="I40" t="b">
-        <v>0</v>
+      <c r="H40" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Oppo+Store+Bantul/@-7.8199142,110.2823455,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5751464646f9:0xece1a8447f4f4b0b!8m2!3d-7.829851!4d110.3537971!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEQY2VsbF9waG9uZV9zdG9yZeABAA!16s%2Fg%2F11rvbk27tk?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J40" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Oppo+Store+Bantul/@-7.8199142,110.2823455,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5751464646f9:0xece1a8447f4f4b0b!8m2!3d-7.829851!4d110.3537971!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEQY2VsbF9waG9uZV9zdG9yZeABAA!16s%2Fg%2F11rvbk27tk?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -2038,25 +1994,24 @@
           <t>0856-4383-7538</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
+      <c r="E41" t="n">
+        <v>5</v>
+      </c>
       <c r="F41" t="n">
-        <v>5</v>
+        <v>-7.918794</v>
       </c>
       <c r="G41" t="n">
-        <v>-7.918794</v>
-      </c>
-      <c r="H41" t="n">
         <v>110.37759</v>
       </c>
-      <c r="I41" t="b">
-        <v>0</v>
-      </c>
-      <c r="J41" t="inlineStr">
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Toko+WS+Imogiri/@-7.9187943,110.3054923,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a55aaa42b4b73:0xae23bae5382ea507!8m2!3d-7.9187943!4d110.3775901!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVUjRaM1UyYldsM1JSQULgAQD6AQQIABAs!16s%2Fg%2F11cs3vfftp?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2075,25 +2030,24 @@
           <t>(0274) 2810667</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
+      <c r="E42" t="n">
+        <v>3.9</v>
+      </c>
       <c r="F42" t="n">
-        <v>3.9</v>
+        <v>-7.797058</v>
       </c>
       <c r="G42" t="n">
-        <v>-7.797058</v>
-      </c>
-      <c r="H42" t="n">
         <v>110.36876</v>
       </c>
-      <c r="I42" t="b">
-        <v>0</v>
-      </c>
-      <c r="J42" t="inlineStr">
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Toko+Sarang+Semut/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a578797a24fc1:0xa8eb0c7a0b4c0b7!8m2!3d-7.797058!4d110.36876!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWySAQp3aG9sZXNhbGVy4AEA!16s%2Fg%2F1pzxbb60f?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2112,25 +2066,24 @@
           <t>0811-2651-692</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
+      <c r="E43" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F43" t="n">
-        <v>4.8</v>
+        <v>-7.786703</v>
       </c>
       <c r="G43" t="n">
-        <v>-7.786703</v>
-      </c>
-      <c r="H43" t="n">
         <v>110.366482</v>
       </c>
-      <c r="I43" t="b">
-        <v>0</v>
-      </c>
-      <c r="J43" t="inlineStr">
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Oleh-Oleh+Jogja+Istimewa+Pulpa/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a590120aa7637:0xd86920e9d406f52b!8m2!3d-7.7867027!4d110.3664817!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F11khkp72bh?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2149,25 +2102,24 @@
           <t>0897-2700-234</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
+      <c r="E44" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F44" t="n">
-        <v>4.6</v>
+        <v>-7.829819</v>
       </c>
       <c r="G44" t="n">
-        <v>-7.829819</v>
-      </c>
-      <c r="H44" t="n">
         <v>110.353804</v>
       </c>
-      <c r="I44" t="b">
-        <v>0</v>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Xiaomi+bantul+resmi/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57e91497a9c9:0x6f03029561733d74!8m2!3d-7.8298194!4d110.3538037!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgERZWxlY3Ryb25pY3Nfc3RvcmXgAQA!16s%2Fg%2F11q3tf_8yk?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J44" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Xiaomi+bantul+resmi/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57e91497a9c9:0x6f03029561733d74!8m2!3d-7.8298194!4d110.3538037!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgERZWxlY3Ryb25pY3Nfc3RvcmXgAQA!16s%2Fg%2F11q3tf_8yk?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -2194,25 +2146,24 @@
           <t>0878-7878-0251</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="n">
+        <v>4.7</v>
+      </c>
       <c r="F45" t="n">
-        <v>4.7</v>
+        <v>-7.796874</v>
       </c>
       <c r="G45" t="n">
-        <v>-7.796874</v>
-      </c>
-      <c r="H45" t="n">
         <v>110.365442</v>
       </c>
-      <c r="I45" t="b">
-        <v>0</v>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Gemah+Ripah/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57881720aa59:0x5198d2225ea2e7f4!8m2!3d-7.7968741!4d110.3654422!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F1tsgh5_p?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J45" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Gemah+Ripah/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57881720aa59:0x5198d2225ea2e7f4!8m2!3d-7.7968741!4d110.3654422!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F1tsgh5_p?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
         <is>
           <t>seminggu lalu</t>
         </is>
@@ -2231,25 +2182,24 @@
       </c>
       <c r="C46" t="inlineStr"/>
       <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F46" t="n">
-        <v>4.8</v>
+        <v>-7.814663</v>
       </c>
       <c r="G46" t="n">
-        <v>-7.814663</v>
-      </c>
-      <c r="H46" t="n">
         <v>110.355791</v>
       </c>
-      <c r="I46" t="b">
-        <v>0</v>
-      </c>
-      <c r="J46" t="inlineStr">
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Istana+Kacamata/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57326389e9d5:0xab631a5358f3dbcb!8m2!3d-7.8146627!4d110.3557905!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEQc3VuZ2xhc3Nlc19zdG9yZeABAA!16s%2Fg%2F11swv00d2t?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2272,25 +2222,24 @@
           <t>0821-3607-9897</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr"/>
+      <c r="E47" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F47" t="n">
-        <v>4.4</v>
+        <v>-7.819727</v>
       </c>
       <c r="G47" t="n">
-        <v>-7.819727</v>
-      </c>
-      <c r="H47" t="n">
         <v>110.355454</v>
       </c>
-      <c r="I47" t="b">
-        <v>0</v>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/New+Toko+kulit+MgCompany4+%2F+Kulit+Nabati+Jogja)/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57bf8297d28d:0xae4662fccfff69a0!8m2!3d-7.8197269!4d110.3554539!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEWbGVhdGhlcl9nb29kc19zdXBwbGllcuABAA!16s%2Fg%2F11c1tdyy81?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J47" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/New+Toko+kulit+MgCompany4+%2F+Kulit+Nabati+Jogja)/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57bf8297d28d:0xae4662fccfff69a0!8m2!3d-7.8197269!4d110.3554539!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEWbGVhdGhlcl9nb29kc19zdXBwbGllcuABAA!16s%2Fg%2F11c1tdyy81?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -2317,25 +2266,24 @@
           <t>(0274) 583237</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
+      <c r="E48" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F48" t="n">
-        <v>4.6</v>
+        <v>-7.797724</v>
       </c>
       <c r="G48" t="n">
-        <v>-7.797724</v>
-      </c>
-      <c r="H48" t="n">
         <v>110.358647</v>
       </c>
-      <c r="I48" t="b">
-        <v>0</v>
-      </c>
-      <c r="J48" t="inlineStr">
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Bakpia+Pathok+25+Ongko+Joyo/@-7.797058,110.2966622,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5775d40149db:0x54613a618d7b0c14!8m2!3d-7.7977241!4d110.358647!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEPc2hvcHBpbmdfY2VudGVy4AEA!16s%2Fg%2F11sfrydv13?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2358,25 +2306,24 @@
           <t>(0274) 583237</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F49" t="n">
-        <v>4.6</v>
+        <v>-7.915893</v>
       </c>
       <c r="G49" t="n">
-        <v>-7.915893</v>
-      </c>
-      <c r="H49" t="n">
         <v>110.398302</v>
       </c>
-      <c r="I49" t="b">
-        <v>0</v>
-      </c>
-      <c r="J49" t="inlineStr">
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Kampung+Batik+Giriloyo/@-7.9158931,110.3262043,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a545f03793c85:0x1ba72bc2befc109f!8m2!3d-7.9158931!4d110.3983021!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEPY3VsdHVyYWxfY2VudGVy4AEA!16s%2Fg%2F11fxzpzkxr?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2395,25 +2342,24 @@
           <t>(0274) 551888</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr"/>
+      <c r="E50" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F50" t="n">
-        <v>4.3</v>
+        <v>-7.793693</v>
       </c>
       <c r="G50" t="n">
-        <v>-7.793693</v>
-      </c>
-      <c r="H50" t="n">
         <v>110.365896</v>
       </c>
-      <c r="I50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J50" t="inlineStr">
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Dagelan+Pusat+Oleh-Oleh+Khas+Jogja/@-7.7936929,110.2937983,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a58262dad55df:0xded076c1f9d1ac2e!8m2!3d-7.7936929!4d110.3658961!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEFc3RvcmXgAQA!16s%2Fg%2F11bzsd7_x4?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2432,25 +2378,24 @@
           <t>(0274) 372132</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
+      <c r="E51" t="n">
+        <v>5</v>
+      </c>
       <c r="F51" t="n">
-        <v>5</v>
+        <v>-7.814444</v>
       </c>
       <c r="G51" t="n">
-        <v>-7.814444</v>
-      </c>
-      <c r="H51" t="n">
         <v>110.35609</v>
       </c>
-      <c r="I51" t="b">
-        <v>0</v>
+      <c r="H51" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Obat+Gunawan/@-7.7936929,110.2937983,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5794e0dea2fb:0x3596a1d8c0189f98!8m2!3d-7.8144437!4d110.3560902!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEIcGhhcm1hY3maASRDaGREU1VoTk1HOW5TMFZKUTBGblNVUllORnBpYmpWUlJSQULgAQD6AQQIABAo!16s%2Fg%2F11b6d401lf?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J51" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Obat+Gunawan/@-7.7936929,110.2937983,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a5794e0dea2fb:0x3596a1d8c0189f98!8m2!3d-7.8144437!4d110.3560902!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgEIcGhhcm1hY3maASRDaGREU1VoTk1HOW5TMFZKUTBGblNVUllORnBpYmpWUlJSQULgAQD6AQQIABAo!16s%2Fg%2F11b6d401lf?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
         <is>
           <t>3 bulan lalu</t>
         </is>
@@ -2473,25 +2418,24 @@
           <t>(0274) 7409978</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr"/>
+      <c r="E52" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F52" t="n">
-        <v>4.3</v>
+        <v>-7.798645</v>
       </c>
       <c r="G52" t="n">
-        <v>-7.798645</v>
-      </c>
-      <c r="H52" t="n">
         <v>110.351869</v>
       </c>
-      <c r="I52" t="b">
-        <v>0</v>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Kerajinan+Jogja/@-7.7936929,110.2937983,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57f5086f93e7:0x2a4191feac4cbde!8m2!3d-7.7986454!4d110.351869!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgELY3JhZnRfc3RvcmXgAQA!16s%2Fg%2F1pzxdzm9g?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J52" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Kerajinan+Jogja/@-7.7936929,110.2937983,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57f5086f93e7:0x2a4191feac4cbde!8m2!3d-7.7986454!4d110.351869!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgELY3JhZnRfc3RvcmXgAQA!16s%2Fg%2F1pzxdzm9g?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -2514,25 +2458,24 @@
           <t>(0274) 7409978</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr"/>
+      <c r="E53" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F53" t="n">
-        <v>4.3</v>
+        <v>-7.798645</v>
       </c>
       <c r="G53" t="n">
-        <v>-7.798645</v>
-      </c>
-      <c r="H53" t="n">
         <v>110.351869</v>
       </c>
-      <c r="I53" t="b">
-        <v>0</v>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Kerajinan+Jogja/@-7.7936929,110.2937983,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57f5086f93e7:0x2a4191feac4cbde!8m2!3d-7.7986454!4d110.351869!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgELY3JhZnRfc3RvcmXgAQA!16s%2Fg%2F1pzxdzm9g?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J53" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Kerajinan+Jogja/@-7.7936929,110.2937983,13z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Bantul!6e6!3m6!1s0x2e7a57f5086f93e7:0x2a4191feac4cbde!8m2!3d-7.7986454!4d110.351869!15sChVUb2tvIE9sZWggb2xlaCBCYW50dWxaFyIVdG9rbyBvbGVoIG9sZWggYmFudHVskgELY3JhZnRfc3RvcmXgAQA!16s%2Fg%2F1pzxdzm9g?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -2555,25 +2498,24 @@
           <t>0857-2735-4144</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr"/>
+      <c r="E54" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F54" t="n">
-        <v>4.3</v>
+        <v>-7.967295</v>
       </c>
       <c r="G54" t="n">
-        <v>-7.967295</v>
-      </c>
-      <c r="H54" t="n">
         <v>110.616873</v>
       </c>
-      <c r="I54" t="b">
-        <v>0</v>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh-oleh+Khas+Gunungkidul+MBAK+TIWIEK/@-7.9462353,110.5451782,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb4a0755934a3:0x152609c293612e0e!8m2!3d-7.9672948!4d110.6168734!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBXN0b3Jl4AEA!16s%2Fg%2F11bw46y2mh?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J54" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh-oleh+Khas+Gunungkidul+MBAK+TIWIEK/@-7.9462353,110.5451782,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb4a0755934a3:0x152609c293612e0e!8m2!3d-7.9672948!4d110.6168734!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBXN0b3Jl4AEA!16s%2Fg%2F11bw46y2mh?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
         <is>
           <t>23 jam lalu</t>
         </is>
@@ -2596,25 +2538,24 @@
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
+      <c r="E55" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F55" t="n">
-        <v>4.4</v>
+        <v>-7.942925</v>
       </c>
       <c r="G55" t="n">
-        <v>-7.942925</v>
-      </c>
-      <c r="H55" t="n">
         <v>110.579394</v>
       </c>
-      <c r="I55" t="b">
-        <v>0</v>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+SARI+RASA/@-7.9429251,110.507296,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb336613031ef:0x76d3732b39e26011!8m2!3d-7.9429251!4d110.5793938!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F1pzptp80h?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J55" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+SARI+RASA/@-7.9429251,110.507296,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb336613031ef:0x76d3732b39e26011!8m2!3d-7.9429251!4d110.5793938!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F1pzptp80h?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
         <is>
           <t>6 hari lalu</t>
         </is>
@@ -2641,25 +2582,24 @@
           <t>0878-3334-3339</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr"/>
+      <c r="E56" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F56" t="n">
-        <v>4.3</v>
+        <v>-7.979502</v>
       </c>
       <c r="G56" t="n">
-        <v>-7.979502</v>
-      </c>
-      <c r="H56" t="n">
         <v>110.598056</v>
       </c>
-      <c r="I56" t="b">
-        <v>0</v>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+SARI+RASA+2/@-7.9429251,110.507296,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb38f2b4dbfc3:0xf1c6a8811b35255b!8m2!3d-7.9795019!4d110.5980556!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F11tmk2jmhg?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J56" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+SARI+RASA+2/@-7.9429251,110.507296,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb38f2b4dbfc3:0xf1c6a8811b35255b!8m2!3d-7.9795019!4d110.5980556!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F11tmk2jmhg?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
         <is>
           <t>2 hari lalu</t>
         </is>
@@ -2682,25 +2622,24 @@
           <t>0878-3987-0070</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="n">
+        <v>4.2</v>
+      </c>
       <c r="F57" t="n">
-        <v>4.2</v>
+        <v>-7.926332</v>
       </c>
       <c r="G57" t="n">
-        <v>-7.926332</v>
-      </c>
-      <c r="H57" t="n">
         <v>110.564457</v>
       </c>
-      <c r="I57" t="b">
-        <v>0</v>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh+-+Oleh+Pak+Kirun/@-7.9429251,110.507296,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7a4d1eb9345d19:0xe1e8980c7df1458a!8m2!3d-7.9263325!4d110.5644565!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F11c2l1pcv_?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J57" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh+-+Oleh+Pak+Kirun/@-7.9429251,110.507296,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7a4d1eb9345d19:0xe1e8980c7df1458a!8m2!3d-7.9263325!4d110.5644565!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F11c2l1pcv_?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
         <is>
           <t>3 hari lalu</t>
         </is>
@@ -2727,25 +2666,24 @@
           <t>0812-1557-9777</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr"/>
+      <c r="E58" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F58" t="n">
-        <v>4.4</v>
+        <v>-7.963801</v>
       </c>
       <c r="G58" t="n">
-        <v>-7.963801</v>
-      </c>
-      <c r="H58" t="n">
         <v>110.609138</v>
       </c>
-      <c r="I58" t="b">
-        <v>0</v>
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Gathot+Thiwul+Yu+Tum/@-7.9429251,110.507296,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb35b8c70cb47:0x76930c23670446a1!8m2!3d-7.9638009!4d110.6091377!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F11rvtn3gw?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J58" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Gathot+Thiwul+Yu+Tum/@-7.9429251,110.507296,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb35b8c70cb47:0x76930c23670446a1!8m2!3d-7.9638009!4d110.6091377!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F11rvtn3gw?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
         <is>
           <t>2 minggu lalu</t>
         </is>
@@ -2764,25 +2702,24 @@
       </c>
       <c r="C59" t="inlineStr"/>
       <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
+      <c r="E59" t="n">
+        <v>4</v>
+      </c>
       <c r="F59" t="n">
-        <v>4</v>
+        <v>-7.97445</v>
       </c>
       <c r="G59" t="n">
-        <v>-7.97445</v>
-      </c>
-      <c r="H59" t="n">
         <v>110.615792</v>
       </c>
-      <c r="I59" t="b">
-        <v>0</v>
+      <c r="H59" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Oleh+Oleh+Gunungkidul/@-7.9744502,110.543694,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb3238a8f4623:0x83e7cee42645a1ec!8m2!3d-7.9744502!4d110.6157918!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bJIBCWdpZnRfc2hvcOABAA!16s%2Fg%2F11tp29ck__?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J59" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Oleh+Oleh+Gunungkidul/@-7.9744502,110.543694,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb3238a8f4623:0x83e7cee42645a1ec!8m2!3d-7.9744502!4d110.6157918!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bJIBCWdpZnRfc2hvcOABAA!16s%2Fg%2F11tp29ck__?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -2805,25 +2742,24 @@
           <t>0851-0500-1164</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr"/>
+      <c r="E60" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F60" t="n">
-        <v>4.3</v>
+        <v>-7.915947</v>
       </c>
       <c r="G60" t="n">
-        <v>-7.915947</v>
-      </c>
-      <c r="H60" t="n">
         <v>110.556234</v>
       </c>
-      <c r="I60" t="b">
-        <v>0</v>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Yu+Tum+Pusat+Oleh+Oleh/@-7.9159469,110.4841365,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7a4d3661442b9d:0x999be29bba53db7c!8m2!3d-7.9159469!4d110.5562343!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBDWdyb2Nlcnlfc3RvcmWaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVTkNMVWxFWlZaM0VBReABAPoBBAgAEEg!16s%2Fg%2F11f89x2486?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J60" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Yu+Tum+Pusat+Oleh+Oleh/@-7.9159469,110.4841365,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7a4d3661442b9d:0x999be29bba53db7c!8m2!3d-7.9159469!4d110.5562343!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBDWdyb2Nlcnlfc3RvcmWaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVTkNMVWxFWlZaM0VBReABAPoBBAgAEEg!16s%2Fg%2F11f89x2486?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
         <is>
           <t>6 hari lalu</t>
         </is>
@@ -2842,25 +2778,24 @@
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
+      <c r="E61" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F61" t="n">
-        <v>4.4</v>
+        <v>-7.964988</v>
       </c>
       <c r="G61" t="n">
-        <v>-7.964988</v>
-      </c>
-      <c r="H61" t="n">
         <v>110.617672</v>
       </c>
-      <c r="I61" t="b">
-        <v>0</v>
+      <c r="H61" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh-oleh+Gunungkidul+Walang+Goreng+Gareng/@-7.9649885,110.5455746,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb4a09098ba15:0x5a4121bbfffd3b2!8m2!3d-7.9649885!4d110.6176724!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBDnNvdXZlbmlyX3N0b3Jl4AEA!16s%2Fg%2F11b809qzqg?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J61" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh-oleh+Gunungkidul+Walang+Goreng+Gareng/@-7.9649885,110.5455746,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb4a09098ba15:0x5a4121bbfffd3b2!8m2!3d-7.9649885!4d110.6176724!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBDnNvdXZlbmlyX3N0b3Jl4AEA!16s%2Fg%2F11b809qzqg?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -2883,25 +2818,24 @@
           <t>(0274) 392910</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr"/>
+      <c r="E62" t="n">
+        <v>4.7</v>
+      </c>
       <c r="F62" t="n">
-        <v>4.7</v>
+        <v>-7.964212</v>
       </c>
       <c r="G62" t="n">
-        <v>-7.964212</v>
-      </c>
-      <c r="H62" t="n">
         <v>110.605365</v>
       </c>
-      <c r="I62" t="b">
-        <v>0</v>
+      <c r="H62" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bakpia+Pathok+101/@-7.9649885,110.5455746,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb35b5a6ffb81:0xf1f97641b960e596!8m2!3d-7.9642122!4d110.6053647!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBD3Nob3BwaW5nX2NlbnRlcpoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VOVVgxQm1PRFZuUlJBQuABAPoBBAgAEEE!16s%2Fg%2F11f0kxx88d?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J62" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Bakpia+Pathok+101/@-7.9649885,110.5455746,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb35b5a6ffb81:0xf1f97641b960e596!8m2!3d-7.9642122!4d110.6053647!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBD3Nob3BwaW5nX2NlbnRlcpoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VOVVgxQm1PRFZuUlJBQuABAPoBBAgAEEE!16s%2Fg%2F11f0kxx88d?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
         <is>
           <t>seminggu lalu</t>
         </is>
@@ -2924,25 +2858,24 @@
           <t>0813-3260-4081</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F63" t="n">
-        <v>4.3</v>
+        <v>-7.966164</v>
       </c>
       <c r="G63" t="n">
-        <v>-7.966164</v>
-      </c>
-      <c r="H63" t="n">
         <v>110.617002</v>
       </c>
-      <c r="I63" t="b">
-        <v>0</v>
+      <c r="H63" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+Walang+Goreng+Pak+Gareng/@-7.9649885,110.5455746,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb4a07fa55905:0xd7fdbca98bb29f8f!8m2!3d-7.9661642!4d110.6170024!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F11c706xtj_?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J63" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+Walang+Goreng+Pak+Gareng/@-7.9649885,110.5455746,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb4a07fa55905:0xd7fdbca98bb29f8f!8m2!3d-7.9661642!4d110.6170024!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBGRlbGngAQA!16s%2Fg%2F11c706xtj_?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
         <is>
           <t>4 minggu lalu</t>
         </is>
@@ -2969,25 +2902,24 @@
           <t>0821-3763-2307</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F64" t="n">
-        <v>4.6</v>
+        <v>-7.912973</v>
       </c>
       <c r="G64" t="n">
-        <v>-7.912973</v>
-      </c>
-      <c r="H64" t="n">
         <v>110.55487</v>
       </c>
-      <c r="I64" t="b">
-        <v>0</v>
+      <c r="H64" t="b">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Javenir+Pusat+Oleh+-+Oleh+Gunung+Kidul/@-7.9129728,110.4827718,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7a4d9fab4d205f:0xdd4460dccdde6737!8m2!3d-7.9129728!4d110.5548696!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBD3Nob3BwaW5nX2NlbnRlcpoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VSNGJEWjFURzFSUlJBQuABAPoBBAgAEDo!16s%2Fg%2F11sc74ztlp?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J64" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Javenir+Pusat+Oleh+-+Oleh+Gunung+Kidul/@-7.9129728,110.4827718,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7a4d9fab4d205f:0xdd4460dccdde6737!8m2!3d-7.9129728!4d110.5548696!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBD3Nob3BwaW5nX2NlbnRlcpoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VSNGJEWjFURzFSUlJBQuABAPoBBAgAEDo!16s%2Fg%2F11sc74ztlp?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
         <is>
           <t>seminggu lalu</t>
         </is>
@@ -3010,25 +2942,24 @@
           <t>0877-3979-2378</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr"/>
+      <c r="E65" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F65" t="n">
-        <v>4.4</v>
+        <v>-7.966838</v>
       </c>
       <c r="G65" t="n">
-        <v>-7.966838</v>
-      </c>
-      <c r="H65" t="n">
         <v>110.610744</v>
       </c>
-      <c r="I65" t="b">
-        <v>0</v>
+      <c r="H65" t="b">
+        <v>0</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/PEYEK+BU+TATIK/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb35dd6f7dca5:0x9d03cbbe2148e148!8m2!3d-7.9668379!4d110.6107438!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBC3Bhc3RyeV9zaG9w4AEA!16s%2Fg%2F11dxl811t7?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J65" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/PEYEK+BU+TATIK/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb35dd6f7dca5:0x9d03cbbe2148e148!8m2!3d-7.9668379!4d110.6107438!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBC3Bhc3RyeV9zaG9w4AEA!16s%2Fg%2F11dxl811t7?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
         <is>
           <t>8 bulan lalu</t>
         </is>
@@ -3051,25 +2982,24 @@
           <t>0877-3897-8676</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F66" t="n">
-        <v>4.6</v>
+        <v>-7.969265</v>
       </c>
       <c r="G66" t="n">
-        <v>-7.969265</v>
-      </c>
-      <c r="H66" t="n">
         <v>110.60172</v>
       </c>
-      <c r="I66" t="b">
-        <v>0</v>
+      <c r="H66" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/HAN+BAKERY,Toko+Roti+Dan+Kue+Wonosari+Gunungkidul/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb3427efe389f:0x61de2f820200bcf3!8m2!3d-7.9692648!4d110.6017195!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBmJha2VyeeABAA!16s%2Fg%2F11g6xpft8t?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J66" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/HAN+BAKERY,Toko+Roti+Dan+Kue+Wonosari+Gunungkidul/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb3427efe389f:0x61de2f820200bcf3!8m2!3d-7.9692648!4d110.6017195!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBmJha2VyeeABAA!16s%2Fg%2F11g6xpft8t?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -3088,25 +3018,24 @@
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F67" t="n">
-        <v>4.4</v>
+        <v>-7.976498</v>
       </c>
       <c r="G67" t="n">
-        <v>-7.976498</v>
-      </c>
-      <c r="H67" t="n">
         <v>110.611808</v>
       </c>
-      <c r="I67" t="b">
-        <v>0</v>
+      <c r="H67" t="b">
+        <v>0</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sweetes+Shop+Wonosari/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb3c7148520cd:0x3b6d4e1ee285b164!8m2!3d-7.9764976!4d110.6118084!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBDmNsb3RoaW5nX3N0b3Jl4AEA!16s%2Fg%2F11kh8jfglb?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J67" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Sweetes+Shop+Wonosari/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb3c7148520cd:0x3b6d4e1ee285b164!8m2!3d-7.9764976!4d110.6118084!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBDmNsb3RoaW5nX3N0b3Jl4AEA!16s%2Fg%2F11kh8jfglb?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
         <is>
           <t>4 bulan lalu</t>
         </is>
@@ -3125,25 +3054,24 @@
       </c>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="n">
+        <v>3.7</v>
+      </c>
       <c r="F68" t="n">
-        <v>3.7</v>
+        <v>-7.96876</v>
       </c>
       <c r="G68" t="n">
-        <v>-7.96876</v>
-      </c>
-      <c r="H68" t="n">
         <v>110.603487</v>
       </c>
-      <c r="I68" t="b">
-        <v>0</v>
+      <c r="H68" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/NICESO+WONOSARI+GUNUNGKIDUL/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb3a54c76823b:0xe46593680bc887f7!8m2!3d-7.9687601!4d110.603487!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBEWNvbnZlbmllbmNlX3N0b3JlmgEjQ2haRFNVaE5NRzluUzBWSlEwRm5TVU53WjNWdGJHWm5FQUXgAQD6AQQIABA2!16s%2Fg%2F11v3j3s0kn?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J68" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/NICESO+WONOSARI+GUNUNGKIDUL/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb3a54c76823b:0xe46593680bc887f7!8m2!3d-7.9687601!4d110.603487!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBEWNvbnZlbmllbmNlX3N0b3JlmgEjQ2haRFNVaE5NRzluUzBWSlEwRm5TVU53WjNWdGJHWm5FQUXgAQD6AQQIABA2!16s%2Fg%2F11v3j3s0kn?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -3170,25 +3098,24 @@
           <t>0812-2854-3940</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F69" t="n">
-        <v>4.9</v>
+        <v>-7.970281</v>
       </c>
       <c r="G69" t="n">
-        <v>-7.970281</v>
-      </c>
-      <c r="H69" t="n">
         <v>110.617887</v>
       </c>
-      <c r="I69" t="b">
-        <v>0</v>
+      <c r="H69" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Khas+Pizza+Wonosari/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb5696e7c9ff7:0xa2422c7086841f7d!8m2!3d-7.970281!4d110.6178867!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBmJha2VyeeABAA!16s%2Fg%2F11llcw1y2h?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J69" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Khas+Pizza+Wonosari/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb5696e7c9ff7:0xa2422c7086841f7d!8m2!3d-7.970281!4d110.6178867!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBmJha2VyeeABAA!16s%2Fg%2F11llcw1y2h?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
         <is>
           <t>4 hari lalu</t>
         </is>
@@ -3211,25 +3138,24 @@
           <t>0811-3001-546</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr"/>
+      <c r="E70" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F70" t="n">
-        <v>4.3</v>
+        <v>-7.968152</v>
       </c>
       <c r="G70" t="n">
-        <v>-7.968152</v>
-      </c>
-      <c r="H70" t="n">
         <v>110.597701</v>
       </c>
-      <c r="I70" t="b">
-        <v>0</v>
+      <c r="H70" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Lala+Shop+Wonosari/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb362202c48d3:0x427b11a0f99b81f9!8m2!3d-7.9681522!4d110.5977006!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBC3N1cGVybWFya2V0mgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVU5vTVhKcWRHcFJSUkFC4AEA-gEECBcQSQ!16s%2Fg%2F11jt1hrg5d?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J70" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Lala+Shop+Wonosari/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb362202c48d3:0x427b11a0f99b81f9!8m2!3d-7.9681522!4d110.5977006!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBC3N1cGVybWFya2V0mgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVU5vTVhKcWRHcFJSUkFC4AEA-gEECBcQSQ!16s%2Fg%2F11jt1hrg5d?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr">
         <is>
           <t>3 minggu lalu</t>
         </is>
@@ -3252,25 +3178,24 @@
           <t>(0274) 2901263</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr"/>
+      <c r="E71" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F71" t="n">
-        <v>4.3</v>
+        <v>-7.976891</v>
       </c>
       <c r="G71" t="n">
-        <v>-7.976891</v>
-      </c>
-      <c r="H71" t="n">
         <v>110.611863</v>
       </c>
-      <c r="I71" t="b">
-        <v>0</v>
+      <c r="H71" t="b">
+        <v>0</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/TOKO+ANDARU+BALEHARJO/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb36376e5a1d9:0xb0beb0b82170d276!8m2!3d-7.9768906!4d110.6118634!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBD3Nob3BwaW5nX2NlbnRlcpoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VOeGFuUlRkR3RSUlJBQuABAPoBBAgAECs!16s%2Fg%2F11f40grsw2?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J71" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/TOKO+ANDARU+BALEHARJO/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb36376e5a1d9:0xb0beb0b82170d276!8m2!3d-7.9768906!4d110.6118634!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBD3Nob3BwaW5nX2NlbnRlcpoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VOeGFuUlRkR3RSUlJBQuABAPoBBAgAECs!16s%2Fg%2F11f40grsw2?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
         <is>
           <t>3 bulan lalu</t>
         </is>
@@ -3293,25 +3218,24 @@
           <t>0812-2790-0045</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F72" t="n">
-        <v>4.4</v>
+        <v>-7.967307</v>
       </c>
       <c r="G72" t="n">
-        <v>-7.967307</v>
-      </c>
-      <c r="H72" t="n">
         <v>110.603376</v>
       </c>
-      <c r="I72" t="b">
-        <v>0</v>
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Mocca+Toko+Roti+Dan+Kue+Gunungkidul/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb342e82ad0b3:0x198530fc515b9bc5!8m2!3d-7.9673072!4d110.6033761!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBmJha2VyeeABAA!16s%2Fg%2F1pzv74bhg?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J72" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Mocca+Toko+Roti+Dan+Kue+Gunungkidul/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb342e82ad0b3:0x198530fc515b9bc5!8m2!3d-7.9673072!4d110.6033761!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBmJha2VyeeABAA!16s%2Fg%2F1pzv74bhg?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K72" t="inlineStr">
         <is>
           <t>3 bulan lalu</t>
         </is>
@@ -3334,25 +3258,24 @@
           <t>0821-3861-4773</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F73" t="n">
-        <v>4.4</v>
+        <v>-7.965005</v>
       </c>
       <c r="G73" t="n">
-        <v>-7.965005</v>
-      </c>
-      <c r="H73" t="n">
         <v>110.606354</v>
       </c>
-      <c r="I73" t="b">
-        <v>0</v>
+      <c r="H73" t="b">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Niela+Sary+Snack,+Roti+dan+Catering/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb35c95f44611:0xa512a4a4fcc948d3!8m2!3d-7.9650051!4d110.6063544!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBmJha2VyeeABAA!16s%2Fg%2F12hktl84w?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J73" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Niela+Sary+Snack,+Roti+dan+Catering/@-7.9668379,110.538646,13z/data=!4m10!1m2!2m1!1sToko+Oleh+oleh+Gunungkidul!3m6!1s0x2e7bb35c95f44611:0xa512a4a4fcc948d3!8m2!3d-7.9650051!4d110.6063544!15sChpUb2tvIE9sZWggb2xlaCBHdW51bmdraWR1bFocIhp0b2tvIG9sZWggb2xlaCBndW51bmdraWR1bJIBBmJha2VyeeABAA!16s%2Fg%2F12hktl84w?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
         <is>
           <t>3 minggu lalu</t>
         </is>
@@ -3375,21 +3298,20 @@
           <t>0857-2590-7688</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
-      <c r="F74" t="n">
+      <c r="E74" t="n">
         <v>4.5</v>
       </c>
+      <c r="F74" t="inlineStr"/>
       <c r="G74" t="inlineStr"/>
-      <c r="H74" t="inlineStr"/>
-      <c r="I74" t="b">
-        <v>0</v>
+      <c r="H74" t="b">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Oleh+Oleh+Jogja/@-7.805191,110.3423289,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a582633dec295:0x8d7cddebc8d3b8f5!8m2!3d-7.793171!4d110.3655261!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F11g6xr9m0d?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J74" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Oleh+Oleh+Jogja/@-7.805191,110.3423289,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a582633dec295:0x8d7cddebc8d3b8f5!8m2!3d-7.793171!4d110.3655261!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F11g6xr9m0d?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K74" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -3408,21 +3330,20 @@
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
-      <c r="F75" t="n">
+      <c r="E75" t="n">
         <v>5</v>
       </c>
+      <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
-      <c r="H75" t="inlineStr"/>
-      <c r="I75" t="b">
-        <v>0</v>
+      <c r="H75" t="b">
+        <v>0</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Pojok+Oleh-oleh/@-7.805191,110.3423289,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a57a7905a7b4d:0x9bd253f5b3f7e6d9!8m2!3d-7.7977717!4d110.3654242!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEFc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVTkNjV1F0V0RoM1JSQULgAQD6AQQIABAv!16s%2Fg%2F11t5_0ywjp?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J75" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Pojok+Oleh-oleh/@-7.805191,110.3423289,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a57a7905a7b4d:0x9bd253f5b3f7e6d9!8m2!3d-7.7977717!4d110.3654242!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEFc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVTkNjV1F0V0RoM1JSQULgAQD6AQQIABAv!16s%2Fg%2F11t5_0ywjp?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K75" t="inlineStr">
         <is>
           <t>4 bulan lalu</t>
         </is>
@@ -3449,21 +3370,20 @@
           <t>0852-8196-8886</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr"/>
-      <c r="F76" t="n">
+      <c r="E76" t="n">
         <v>5</v>
       </c>
+      <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
-      <c r="H76" t="inlineStr"/>
-      <c r="I76" t="b">
-        <v>0</v>
+      <c r="H76" t="b">
+        <v>0</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bakpia+Pathok+086+Jaya+Oleh-oleh+Khas+Jogja/@-7.7867027,110.3484573,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a598a34b2dd7b:0x6255508db431c7f3!8m2!3d-7.7976244!4d110.3658617!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEPc2hvcHBpbmdfY2VudGVy4AEA!16s%2Fg%2F11qlzkzh5g?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J76" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Bakpia+Pathok+086+Jaya+Oleh-oleh+Khas+Jogja/@-7.7867027,110.3484573,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a598a34b2dd7b:0x6255508db431c7f3!8m2!3d-7.7976244!4d110.3658617!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEPc2hvcHBpbmdfY2VudGVy4AEA!16s%2Fg%2F11qlzkzh5g?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K76" t="inlineStr">
         <is>
           <t>4 hari lalu</t>
         </is>
@@ -3486,21 +3406,20 @@
           <t>(0274) 562985</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr"/>
-      <c r="F77" t="n">
+      <c r="E77" t="n">
         <v>4.5</v>
       </c>
+      <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
-      <c r="H77" t="inlineStr"/>
-      <c r="I77" t="b">
-        <v>0</v>
+      <c r="H77" t="b">
+        <v>0</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh/@-7.7867027,110.3484573,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a58289c4c7c19:0x90bf3e3bd6d7021b!8m2!3d-7.7927108!4d110.3665766!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGGSAQ5zb3V2ZW5pcl9zdG9yZeABAA!16s%2Fg%2F1pzr_74yh?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J77" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh/@-7.7867027,110.3484573,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a58289c4c7c19:0x90bf3e3bd6d7021b!8m2!3d-7.7927108!4d110.3665766!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGGSAQ5zb3V2ZW5pcl9zdG9yZeABAA!16s%2Fg%2F1pzr_74yh?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K77" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -3527,21 +3446,20 @@
           <t>(0274) 588524</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr"/>
-      <c r="F78" t="n">
+      <c r="E78" t="n">
         <v>4.6</v>
       </c>
+      <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
-      <c r="H78" t="inlineStr"/>
-      <c r="I78" t="b">
-        <v>0</v>
+      <c r="H78" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Hamzah+Batik+-+Toko+Batik+dan+Oleh-oleh+Khas+Jogja/@-7.7867027,110.3484573,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a5788f761d221:0x6e56f49ab472d198!8m2!3d-7.7991629!4d110.3647534!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEFc3RvcmXgAQA!16s%2Fg%2F1tf2pnpf?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J78" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Hamzah+Batik+-+Toko+Batik+dan+Oleh-oleh+Khas+Jogja/@-7.7867027,110.3484573,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a5788f761d221:0x6e56f49ab472d198!8m2!3d-7.7991629!4d110.3647534!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEFc3RvcmXgAQA!16s%2Fg%2F1tf2pnpf?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K78" t="inlineStr">
         <is>
           <t>12 menit lalu</t>
         </is>
@@ -3564,21 +3482,20 @@
           <t>0812-7318-3131</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr"/>
-      <c r="F79" t="n">
+      <c r="E79" t="n">
         <v>4.4</v>
       </c>
+      <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr"/>
-      <c r="H79" t="inlineStr"/>
-      <c r="I79" t="b">
-        <v>0</v>
+      <c r="H79" t="b">
+        <v>0</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/%22TOKO+KITA+2%22+Oleh-Oleh+Khas+Jogja/@-7.7867027,110.3484573,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a579423539ab1:0x700fc2d009769e7a!8m2!3d-7.8013908!4d110.3620519!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEGYmFrZXJ54AEA!16s%2Fg%2F11t8kcj0rs?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J79" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/%22TOKO+KITA+2%22+Oleh-Oleh+Khas+Jogja/@-7.7867027,110.3484573,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a579423539ab1:0x700fc2d009769e7a!8m2!3d-7.8013908!4d110.3620519!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEGYmFrZXJ54AEA!16s%2Fg%2F11t8kcj0rs?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -3601,21 +3518,20 @@
           <t>(0274) 377295</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
-      <c r="F80" t="n">
+      <c r="E80" t="n">
         <v>4.4</v>
       </c>
+      <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
-      <c r="H80" t="inlineStr"/>
-      <c r="I80" t="b">
-        <v>0</v>
+      <c r="H80" t="b">
+        <v>0</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Aroma+Yogyakarta/@-7.8069491,110.3513379,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a579a2bd999b9:0x5c909ec051c8375d!8m2!3d-7.8069491!4d110.3693623!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgETYmFraW5nX3N1cHBseV9zdG9yZeABAA!16s%2Fg%2F1hc18b3xd?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J80" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Aroma+Yogyakarta/@-7.8069491,110.3513379,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a579a2bd999b9:0x5c909ec051c8375d!8m2!3d-7.8069491!4d110.3693623!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgETYmFraW5nX3N1cHBseV9zdG9yZeABAA!16s%2Fg%2F1hc18b3xd?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -3642,21 +3558,20 @@
           <t>0813-2073-6867</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr"/>
-      <c r="F81" t="n">
+      <c r="E81" t="n">
         <v>4.8</v>
       </c>
+      <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
-      <c r="H81" t="inlineStr"/>
-      <c r="I81" t="b">
-        <v>0</v>
+      <c r="H81" t="b">
+        <v>0</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Oleh-oleh+Podjok+Wisata/@-7.7864943,110.348813,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a5961c2969963:0x73fedf7c39372a74!8m2!3d-7.7864943!4d110.3668374!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEPc2hvcHBpbmdfY2VudGVy4AEA!16s%2Fg%2F11h00d0yrz?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J81" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Oleh-oleh+Podjok+Wisata/@-7.7864943,110.348813,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a5961c2969963:0x73fedf7c39372a74!8m2!3d-7.7864943!4d110.3668374!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEPc2hvcHBpbmdfY2VudGVy4AEA!16s%2Fg%2F11h00d0yrz?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
         <is>
           <t>8 bulan lalu</t>
         </is>
@@ -3679,21 +3594,20 @@
           <t>(0274) 588143</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr"/>
-      <c r="F82" t="n">
+      <c r="E82" t="n">
         <v>4.6</v>
       </c>
+      <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
-      <c r="H82" t="inlineStr"/>
-      <c r="I82" t="b">
-        <v>0</v>
+      <c r="H82" t="b">
+        <v>0</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Camilan+Dan+Snack+Bu+Wiwik+Yogyakarta/@-7.7864943,110.348813,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a582bcd6e5c51:0xfb2c44dee37ba248!8m2!3d-7.7929786!4d110.3733971!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgENZ3JvY2VyeV9zdG9yZZoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VOaFoyRmhNM0ZSUlJBQuABAPoBBQj7AhA3!16s%2Fg%2F1hm2sny6v?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J82" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Camilan+Dan+Snack+Bu+Wiwik+Yogyakarta/@-7.7864943,110.348813,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a582bcd6e5c51:0xfb2c44dee37ba248!8m2!3d-7.7929786!4d110.3733971!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgENZ3JvY2VyeV9zdG9yZZoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VOaFoyRmhNM0ZSUlJBQuABAPoBBQj7AhA3!16s%2Fg%2F1hm2sny6v?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
         <is>
           <t>1 hari lalu</t>
         </is>
@@ -3716,21 +3630,20 @@
           <t>0812-1585-6232</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr"/>
-      <c r="F83" t="n">
+      <c r="E83" t="n">
         <v>4.4</v>
       </c>
+      <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
-      <c r="I83" t="b">
-        <v>0</v>
+      <c r="H83" t="b">
+        <v>0</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Raden+Oleh-Oleh+Jogja+-+Cabang+Ahmad+Dahlan/@-7.7864943,110.348813,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a578040e683b9:0xdca6ec59bd515a23!8m2!3d-7.8012427!4d110.363371!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEGYmFrZXJ54AEA!16s%2Fg%2F11jzrdp0qs?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J83" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Raden+Oleh-Oleh+Jogja+-+Cabang+Ahmad+Dahlan/@-7.7864943,110.348813,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a578040e683b9:0xdca6ec59bd515a23!8m2!3d-7.8012427!4d110.363371!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEGYmFrZXJ54AEA!16s%2Fg%2F11jzrdp0qs?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -3753,21 +3666,20 @@
           <t>(0274) 379625</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr"/>
-      <c r="F84" t="n">
+      <c r="E84" t="n">
         <v>4.5</v>
       </c>
+      <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
-      <c r="H84" t="inlineStr"/>
-      <c r="I84" t="b">
-        <v>0</v>
+      <c r="H84" t="b">
+        <v>0</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Batik+Wisnu/@-7.8035408,110.3484831,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a5785992a1441:0x601fc1a572ff7d09!8m2!3d-7.8035408!4d110.3665075!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEOY2xvdGhpbmdfc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVTjRlbGt0WjNCQlJSQULgAQD6AQQIABBI!16s%2Fg%2F1pzq3l8p0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J84" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Batik+Wisnu/@-7.8035408,110.3484831,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a5785992a1441:0x601fc1a572ff7d09!8m2!3d-7.8035408!4d110.3665075!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEOY2xvdGhpbmdfc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVTjRlbGt0WjNCQlJSQULgAQD6AQQIABBI!16s%2Fg%2F1pzq3l8p0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
         <is>
           <t>30 menit lalu</t>
         </is>
@@ -3786,21 +3698,20 @@
       </c>
       <c r="C85" t="inlineStr"/>
       <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
-      <c r="F85" t="n">
+      <c r="E85" t="n">
         <v>4.7</v>
       </c>
+      <c r="F85" t="inlineStr"/>
       <c r="G85" t="inlineStr"/>
-      <c r="H85" t="inlineStr"/>
-      <c r="I85" t="b">
-        <v>0</v>
+      <c r="H85" t="b">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Raminten+Souvenir/@-7.8035408,110.3484831,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a57de3a5ced21:0x39c5fe038b0f2a37!8m2!3d-7.7991633!4d110.364771!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEOc291dmVuaXJfc3RvcmWaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVUktNWFV5WTA1UkVBReABAPoBBAgAEEE!16s%2Fg%2F11gjzmgvjc?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J85" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Raminten+Souvenir/@-7.8035408,110.3484831,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a57de3a5ced21:0x39c5fe038b0f2a37!8m2!3d-7.7991633!4d110.364771!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEOc291dmVuaXJfc3RvcmWaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVUktNWFV5WTA1UkVBReABAPoBBAgAEEE!16s%2Fg%2F11gjzmgvjc?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
         <is>
           <t>4 minggu lalu</t>
         </is>
@@ -3823,21 +3734,20 @@
           <t>0818-1888-8863</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr"/>
-      <c r="F86" t="n">
+      <c r="E86" t="n">
         <v>4.6</v>
       </c>
+      <c r="F86" t="inlineStr"/>
       <c r="G86" t="inlineStr"/>
-      <c r="H86" t="inlineStr"/>
-      <c r="I86" t="b">
-        <v>0</v>
+      <c r="H86" t="b">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bakpia+Wong+Keraton/@-7.7909742,110.33537,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a5818b14eeda1:0x4cf80887f0f34dc1!8m2!3d-7.7909742!4d110.3533944!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEPc2hvcHBpbmdfY2VudGVy4AEA!16s%2Fg%2F11gfgm6x56?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J86" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Bakpia+Wong+Keraton/@-7.7909742,110.33537,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a5818b14eeda1:0x4cf80887f0f34dc1!8m2!3d-7.7909742!4d110.3533944!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEPc2hvcHBpbmdfY2VudGVy4AEA!16s%2Fg%2F11gfgm6x56?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K86" t="inlineStr">
         <is>
           <t>1 hari lalu</t>
         </is>
@@ -3860,21 +3770,20 @@
           <t>(0274) 373371</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr"/>
-      <c r="F87" t="n">
+      <c r="E87" t="n">
         <v>4.3</v>
       </c>
+      <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
-      <c r="H87" t="inlineStr"/>
-      <c r="I87" t="b">
-        <v>0</v>
+      <c r="H87" t="b">
+        <v>0</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Prapanca+Batik+dan+Kerajinan/@-7.8021258,110.346382,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a578f3b1116ad:0x295a9fb698e403e4!8m2!3d-7.8021258!4d110.3644064!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F1tdlrdgr?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J87" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Prapanca+Batik+dan+Kerajinan/@-7.8021258,110.346382,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kota+Yogyakarta!6e6!3m6!1s0x2e7a578f3b1116ad:0x295a9fb698e403e4!8m2!3d-7.8021258!4d110.3644064!15sCh5Ub2tvIE9sZWggb2xlaCBLb3RhIFlvZ3lha2FydGFaICIedG9rbyBvbGVoIG9sZWgga290YSB5b2d5YWthcnRhkgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F1tdlrdgr?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoJLDEwMjExMjM0SAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -3901,21 +3810,20 @@
           <t>0851-0140-4222</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr"/>
-      <c r="F88" t="n">
+      <c r="E88" t="n">
         <v>4.5</v>
       </c>
+      <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
-      <c r="H88" t="inlineStr"/>
-      <c r="I88" t="b">
-        <v>0</v>
-      </c>
-      <c r="J88" t="inlineStr">
+      <c r="H88" t="b">
+        <v>0</v>
+      </c>
+      <c r="I88" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Toko+Oleh-oleh+Wingko+SusiloWati/@-7.865617,109.870864,11z/data=!4m13!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m8!1s0x2e7afb3f275a17ed:0x253a36da360ccb1!8m2!3d-7.865617!4d110.1592551!9m1!1b1!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F1pzs4s_t4?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3930,25 +3838,24 @@
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F89" t="n">
-        <v>4.4</v>
+        <v>-7.865678</v>
       </c>
       <c r="G89" t="n">
-        <v>-7.865678</v>
-      </c>
-      <c r="H89" t="n">
         <v>110.158167</v>
       </c>
-      <c r="I89" t="b">
-        <v>0</v>
+      <c r="H89" t="b">
+        <v>0</v>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Oleh-Oleh+Khas+Yogya+Toko+Hana/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb3f2aef5607:0x186333bbb997dd87!8m2!3d-7.8656782!4d110.158167!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11b6syl69q?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J89" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Oleh-Oleh+Khas+Yogya+Toko+Hana/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb3f2aef5607:0x186333bbb997dd87!8m2!3d-7.8656782!4d110.158167!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11b6syl69q?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -3971,25 +3878,24 @@
           <t>(0274) 773417</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr"/>
+      <c r="E90" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F90" t="n">
-        <v>4.6</v>
+        <v>-7.86169</v>
       </c>
       <c r="G90" t="n">
-        <v>-7.86169</v>
-      </c>
-      <c r="H90" t="n">
         <v>110.157822</v>
       </c>
-      <c r="I90" t="b">
-        <v>0</v>
+      <c r="H90" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Fajar+Baru+LUMBUNG+OLEH+OLEH/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb3b86f89c4f:0x2932ae20a398449e!8m2!3d-7.8616904!4d110.1578218!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBCmZvb2Rfc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVUnFhbEJ1TlRWblJSQULgAQD6AQQIJBAn!16s%2Fg%2F11b6x4gtyf?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J90" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Fajar+Baru+LUMBUNG+OLEH+OLEH/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb3b86f89c4f:0x2932ae20a398449e!8m2!3d-7.8616904!4d110.1578218!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBCmZvb2Rfc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVUnFhbEJ1TlRWblJSQULgAQD6AQQIJBAn!16s%2Fg%2F11b6x4gtyf?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -4012,25 +3918,24 @@
           <t>0822-2660-1971</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr"/>
+      <c r="E91" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F91" t="n">
-        <v>4.8</v>
+        <v>-7.877223</v>
       </c>
       <c r="G91" t="n">
-        <v>-7.877223</v>
-      </c>
-      <c r="H91" t="n">
         <v>110.133803</v>
       </c>
-      <c r="I91" t="b">
-        <v>0</v>
+      <c r="H91" t="b">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/TokoMu+Kulon+Progo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae59d8f52f233:0xfc1e9f580b3ce836!8m2!3d-7.8772232!4d110.1338032!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBEWNvbnZlbmllbmNlX3N0b3JlmgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVVJHY25WcFZIcFJSUkFC4AEA-gEECAAQPQ!16s%2Fg%2F11pwrj253l?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J91" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/TokoMu+Kulon+Progo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae59d8f52f233:0xfc1e9f580b3ce836!8m2!3d-7.8772232!4d110.1338032!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBEWNvbnZlbmllbmNlX3N0b3JlmgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVVJHY25WcFZIcFJSUkFC4AEA-gEECAAQPQ!16s%2Fg%2F11pwrj253l?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
         <is>
           <t>4 bulan lalu</t>
         </is>
@@ -4053,25 +3958,24 @@
         </is>
       </c>
       <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
+      <c r="E92" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F92" t="n">
-        <v>4.8</v>
+        <v>-7.864287</v>
       </c>
       <c r="G92" t="n">
-        <v>-7.864287</v>
-      </c>
-      <c r="H92" t="n">
         <v>110.160441</v>
       </c>
-      <c r="I92" t="b">
-        <v>0</v>
+      <c r="H92" t="b">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Istana+Oleh-Oleh+Omah+Gedhang+JogjaKu/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb25e2463f31:0x45e71a8d4f3e1b72!8m2!3d-7.8642869!4d110.1604412!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBC3N1cGVybWFya2V04AEA!16s%2Fg%2F11klr1lh98?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J92" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Istana+Oleh-Oleh+Omah+Gedhang+JogjaKu/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb25e2463f31:0x45e71a8d4f3e1b72!8m2!3d-7.8642869!4d110.1604412!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBC3N1cGVybWFya2V04AEA!16s%2Fg%2F11klr1lh98?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -4098,25 +4002,24 @@
           <t>0852-0554-0141</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr"/>
+      <c r="E93" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F93" t="n">
-        <v>4.5</v>
+        <v>-7.864466</v>
       </c>
       <c r="G93" t="n">
-        <v>-7.864466</v>
-      </c>
-      <c r="H93" t="n">
         <v>110.144184</v>
       </c>
-      <c r="I93" t="b">
-        <v>0</v>
+      <c r="H93" t="b">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Moa+and+Co+(+oleh+-+oleh+kulon+progo+)/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb143335a85f:0x6d9801d271fba784!8m2!3d-7.864466!4d110.1441838!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDnNvdXZlbmlyX3N0b3Jl4AEA!16s%2Fg%2F11h07fcp_p?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J93" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Moa+and+Co+(+oleh+-+oleh+kulon+progo+)/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb143335a85f:0x6d9801d271fba784!8m2!3d-7.864466!4d110.1441838!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDnNvdXZlbmlyX3N0b3Jl4AEA!16s%2Fg%2F11h07fcp_p?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K93" t="inlineStr">
         <is>
           <t>4 tahun lalu</t>
         </is>
@@ -4143,25 +4046,24 @@
           <t>0898-4810-000</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr"/>
+      <c r="E94" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F94" t="n">
-        <v>4.9</v>
+        <v>-7.864998</v>
       </c>
       <c r="G94" t="n">
-        <v>-7.864998</v>
-      </c>
-      <c r="H94" t="n">
         <v>110.157262</v>
       </c>
-      <c r="I94" t="b">
-        <v>0</v>
+      <c r="H94" t="b">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Cokelat+Makaryo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb498f622e2f:0x6b2f31e556dbab0a!8m2!3d-7.8649982!4d110.157262!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDmNob2NvbGF0ZV9zaG9w4AEA!16s%2Fg%2F11gxjwb52b?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J94" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Cokelat+Makaryo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb498f622e2f:0x6b2f31e556dbab0a!8m2!3d-7.8649982!4d110.157262!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDmNob2NvbGF0ZV9zaG9w4AEA!16s%2Fg%2F11gxjwb52b?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K94" t="inlineStr">
         <is>
           <t>3 minggu lalu</t>
         </is>
@@ -4184,25 +4086,24 @@
           <t>0815-7989-746</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr"/>
+      <c r="E95" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F95" t="n">
-        <v>4.5</v>
+        <v>-7.851259</v>
       </c>
       <c r="G95" t="n">
-        <v>-7.851259</v>
-      </c>
-      <c r="H95" t="n">
         <v>110.158916</v>
       </c>
-      <c r="I95" t="b">
-        <v>0</v>
+      <c r="H95" t="b">
+        <v>0</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Wingko+Suci+Harwati/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb21382d0e41:0xd1c8bbaa2b1ba384!8m2!3d-7.8512587!4d110.1589156!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBE25hdHVyYWxfZm9vZHNfc3RvcmXgAQA!16s%2Fg%2F11cmrtsf91?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J95" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Wingko+Suci+Harwati/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb21382d0e41:0xd1c8bbaa2b1ba384!8m2!3d-7.8512587!4d110.1589156!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBE25hdHVyYWxfZm9vZHNfc3RvcmXgAQA!16s%2Fg%2F11cmrtsf91?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K95" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -4225,25 +4126,24 @@
           <t>0877-8150-0081</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr"/>
+      <c r="E96" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F96" t="n">
-        <v>4.5</v>
+        <v>-7.890045</v>
       </c>
       <c r="G96" t="n">
-        <v>-7.890045</v>
-      </c>
-      <c r="H96" t="n">
         <v>110.103103</v>
       </c>
-      <c r="I96" t="b">
-        <v>0</v>
+      <c r="H96" t="b">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/J%26C+Pusat+Oleh+Oleh+Khas+Jogja+2/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae555846a66f7:0x7c7f3a857084d7e4!8m2!3d-7.8900455!4d110.1031029!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDWdlbmVyYWxfc3RvcmXgAQA!16s%2Fg%2F11tjg7r1ym?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J96" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/J%26C+Pusat+Oleh+Oleh+Khas+Jogja+2/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae555846a66f7:0x7c7f3a857084d7e4!8m2!3d-7.8900455!4d110.1031029!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDWdlbmVyYWxfc3RvcmXgAQA!16s%2Fg%2F11tjg7r1ym?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr">
         <is>
           <t>6 hari lalu</t>
         </is>
@@ -4266,25 +4166,24 @@
           <t>0812-3828-3363</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
+      <c r="E97" t="n">
+        <v>5</v>
+      </c>
       <c r="F97" t="n">
-        <v>5</v>
+        <v>-7.892219</v>
       </c>
       <c r="G97" t="n">
-        <v>-7.892219</v>
-      </c>
-      <c r="H97" t="n">
         <v>110.128218</v>
       </c>
-      <c r="I97" t="b">
-        <v>0</v>
+      <c r="H97" t="b">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+Khas+Jogja/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae58a9f68fa27:0x7e468ef3b248d2f5!8m2!3d-7.8922186!4d110.1282175!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11t9n5kc4x?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J97" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh-Oleh+Khas+Jogja/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae58a9f68fa27:0x7e468ef3b248d2f5!8m2!3d-7.8922186!4d110.1282175!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11t9n5kc4x?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K97" t="inlineStr">
         <is>
           <t>4 minggu lalu</t>
         </is>
@@ -4311,25 +4210,24 @@
           <t>0819-3176-4176</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr"/>
+      <c r="E98" t="n">
+        <v>5</v>
+      </c>
       <c r="F98" t="n">
-        <v>5</v>
+        <v>-7.898907</v>
       </c>
       <c r="G98" t="n">
-        <v>-7.898907</v>
-      </c>
-      <c r="H98" t="n">
         <v>110.058798</v>
       </c>
-      <c r="I98" t="b">
-        <v>0</v>
+      <c r="H98" t="b">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Mawar+Pusat+Oleh-oleh+YIA/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae312cb88ef2d:0xd4ab79d5f2505da8!8m2!3d-7.8989074!4d110.0587981!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBCWdpZnRfc2hvcOABAA!16s%2Fg%2F11rqnq0q7d?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J98" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Mawar+Pusat+Oleh-oleh+YIA/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae312cb88ef2d:0xd4ab79d5f2505da8!8m2!3d-7.8989074!4d110.0587981!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBCWdpZnRfc2hvcOABAA!16s%2Fg%2F11rqnq0q7d?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K98" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -4352,25 +4250,24 @@
           <t>(0274) 773880</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr"/>
+      <c r="E99" t="n">
+        <v>3.9</v>
+      </c>
       <c r="F99" t="n">
-        <v>3.9</v>
+        <v>-7.866917</v>
       </c>
       <c r="G99" t="n">
-        <v>-7.866917</v>
-      </c>
-      <c r="H99" t="n">
         <v>110.15011</v>
       </c>
-      <c r="I99" t="b">
-        <v>0</v>
+      <c r="H99" t="b">
+        <v>0</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+Oleh-oleh+%26+Kerajinan+Khas+Jogja+Wates+Kulon+Progo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb37ca733bbf:0xb11476ae2ddbcff1!8m2!3d-7.8669169!4d110.15011!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBGZvb2SaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVTkdaelJ0VTAxUkVBReABAPoBBAgAECE!16s%2Fg%2F11b6rx_7k0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J99" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+Oleh-oleh+%26+Kerajinan+Khas+Jogja+Wates+Kulon+Progo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb37ca733bbf:0xb11476ae2ddbcff1!8m2!3d-7.8669169!4d110.15011!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBGZvb2SaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVTkdaelJ0VTAxUkVBReABAPoBBAgAECE!16s%2Fg%2F11b6rx_7k0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K99" t="inlineStr">
         <is>
           <t>3 bulan lalu</t>
         </is>
@@ -4393,25 +4290,24 @@
           <t>0818-0411-7440</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr"/>
+      <c r="E100" t="n">
+        <v>4.7</v>
+      </c>
       <c r="F100" t="n">
-        <v>4.7</v>
+        <v>-7.859608</v>
       </c>
       <c r="G100" t="n">
-        <v>-7.859608</v>
-      </c>
-      <c r="H100" t="n">
         <v>110.174413</v>
       </c>
-      <c r="I100" t="b">
-        <v>0</v>
+      <c r="H100" t="b">
+        <v>0</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bakpia+Prasojo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb840b14d2d3:0x8585327eebbe5871!8m2!3d-7.8596082!4d110.1744131!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11st6fxd1n?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J100" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Bakpia+Prasojo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb840b14d2d3:0x8585327eebbe5871!8m2!3d-7.8596082!4d110.1744131!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11st6fxd1n?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K100" t="inlineStr">
         <is>
           <t>3 hari lalu</t>
         </is>
@@ -4434,25 +4330,24 @@
           <t>(0274) 773925</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr"/>
+      <c r="E101" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F101" t="n">
-        <v>4.4</v>
+        <v>-7.802965</v>
       </c>
       <c r="G101" t="n">
-        <v>-7.802965</v>
-      </c>
-      <c r="H101" t="n">
         <v>110.164507</v>
       </c>
-      <c r="I101" t="b">
-        <v>0</v>
+      <c r="H101" t="b">
+        <v>0</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Wingko+'Susilowati'/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7af00955802fb9:0xddae99169a0c6b80!8m2!3d-7.8029647!4d110.1645069!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBCmZvb2Rfc3RvcmXgAQA!16s%2Fg%2F1pzvqxc_j?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J101" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Wingko+'Susilowati'/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7af00955802fb9:0xddae99169a0c6b80!8m2!3d-7.8029647!4d110.1645069!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBCmZvb2Rfc3RvcmXgAQA!16s%2Fg%2F1pzvqxc_j?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K101" t="inlineStr">
         <is>
           <t>10 jam lalu</t>
         </is>
@@ -4475,25 +4370,24 @@
           <t>0822-4211-1881</t>
         </is>
       </c>
-      <c r="E102" t="inlineStr"/>
+      <c r="E102" t="n">
+        <v>5</v>
+      </c>
       <c r="F102" t="n">
-        <v>5</v>
+        <v>-7.856814</v>
       </c>
       <c r="G102" t="n">
-        <v>-7.856814</v>
-      </c>
-      <c r="H102" t="n">
         <v>110.160849</v>
       </c>
-      <c r="I102" t="b">
-        <v>0</v>
+      <c r="H102" t="b">
+        <v>0</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Meat+Nata+Wates+(Meat+Shop+-+Seafood+-+Frozen+Food)+Kulon+Progo+Yogyakarta/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afba50022c98f:0x7bc21bf88455a0a9!8m2!3d-7.8568142!4d110.1608486!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBFWdvdXJtZXRfZ3JvY2VyeV9zdG9yZeABAA!16s%2Fg%2F11rbm35mp3?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J102" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Meat+Nata+Wates+(Meat+Shop+-+Seafood+-+Frozen+Food)+Kulon+Progo+Yogyakarta/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afba50022c98f:0x7bc21bf88455a0a9!8m2!3d-7.8568142!4d110.1608486!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBFWdvdXJtZXRfZ3JvY2VyeV9zdG9yZeABAA!16s%2Fg%2F11rbm35mp3?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K102" t="inlineStr">
         <is>
           <t>19 jam lalu</t>
         </is>
@@ -4512,25 +4406,24 @@
       </c>
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
+      <c r="E103" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F103" t="n">
-        <v>4.8</v>
+        <v>-7.863514</v>
       </c>
       <c r="G103" t="n">
-        <v>-7.863514</v>
-      </c>
-      <c r="H103" t="n">
         <v>110.151552</v>
       </c>
-      <c r="I103" t="b">
-        <v>0</v>
+      <c r="H103" t="b">
+        <v>0</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Siliwangi+Bolu+Kukus+Wates,+Kulon+Progo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb5e885ce547:0xe9060e7a1377f380!8m2!3d-7.8635139!4d110.1515516!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11stq9nvtt?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J103" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Siliwangi+Bolu+Kukus+Wates,+Kulon+Progo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb5e885ce547:0xe9060e7a1377f380!8m2!3d-7.8635139!4d110.1515516!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11stq9nvtt?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K103" t="inlineStr">
         <is>
           <t>3 minggu lalu</t>
         </is>
@@ -4549,25 +4442,24 @@
       </c>
       <c r="C104" t="inlineStr"/>
       <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
+      <c r="E104" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F104" t="n">
-        <v>4.9</v>
+        <v>-7.866014</v>
       </c>
       <c r="G104" t="n">
-        <v>-7.866014</v>
-      </c>
-      <c r="H104" t="n">
         <v>110.149229</v>
       </c>
-      <c r="I104" t="b">
-        <v>0</v>
+      <c r="H104" t="b">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/TOKO+OLEH2+UMKM+KULON+PROGO+%26+PUSAT+JAJANAN+PASAR+UBERMAH/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb0060dda7a7:0xcc503f2f3a37cafe!8m2!3d-7.8660142!4d110.1492292!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBC3N1cGVybWFya2V0mgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVU5mTVhCRFVYaFJSUkFC4AEA-gEECAAQRw!16s%2Fg%2F11ybdwj4n5?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J104" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/TOKO+OLEH2+UMKM+KULON+PROGO+%26+PUSAT+JAJANAN+PASAR+UBERMAH/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb0060dda7a7:0xcc503f2f3a37cafe!8m2!3d-7.8660142!4d110.1492292!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBC3N1cGVybWFya2V0mgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVU5mTVhCRFVYaFJSUkFC4AEA-gEECAAQRw!16s%2Fg%2F11ybdwj4n5?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K104" t="inlineStr">
         <is>
           <t>2 minggu lalu</t>
         </is>
@@ -4586,25 +4478,24 @@
       </c>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
+      <c r="E105" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F105" t="n">
-        <v>4.6</v>
+        <v>-7.835808</v>
       </c>
       <c r="G105" t="n">
-        <v>-7.835808</v>
-      </c>
-      <c r="H105" t="n">
         <v>110.167098</v>
       </c>
-      <c r="I105" t="b">
-        <v>0</v>
+      <c r="H105" t="b">
+        <v>0</v>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Bela/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afae88a0dccb7:0x3154f45f0b5fc115!8m2!3d-7.8358081!4d110.1670979!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBXN0b3JlmgEjQ2haRFNVaE5NRzluUzBWSlEwRm5TVU5LYkhCMk5HUjNFQUXgAQD6AQQIABBF!16s%2Fg%2F11bzrpk04_?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J105" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Bela/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afae88a0dccb7:0x3154f45f0b5fc115!8m2!3d-7.8358081!4d110.1670979!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBXN0b3JlmgEjQ2haRFNVaE5NRzluUzBWSlEwRm5TVU5LYkhCMk5HUjNFQUXgAQD6AQQIABBF!16s%2Fg%2F11bzrpk04_?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K105" t="inlineStr">
         <is>
           <t>4 bulan lalu</t>
         </is>
@@ -4631,25 +4522,24 @@
           <t>0821-6468-7799</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr"/>
+      <c r="E106" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F106" t="n">
-        <v>4.5</v>
+        <v>-7.863275</v>
       </c>
       <c r="G106" t="n">
-        <v>-7.863275</v>
-      </c>
-      <c r="H106" t="n">
         <v>110.15755</v>
       </c>
-      <c r="I106" t="b">
-        <v>0</v>
+      <c r="H106" t="b">
+        <v>0</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Papa+Cookies+Kulon+Progo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afbab8ff53a1b:0x285b60ece002a909!8m2!3d-7.863275!4d110.1575499!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11jm73l3ht?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J106" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Papa+Cookies+Kulon+Progo/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afbab8ff53a1b:0x285b60ece002a909!8m2!3d-7.863275!4d110.1575499!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBmJha2VyeeABAA!16s%2Fg%2F11jm73l3ht?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K106" t="inlineStr">
         <is>
           <t>4 hari lalu</t>
         </is>
@@ -4672,25 +4562,24 @@
           <t>0852-9342-3104</t>
         </is>
       </c>
-      <c r="E107" t="inlineStr"/>
+      <c r="E107" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F107" t="n">
-        <v>4.4</v>
+        <v>-7.83739</v>
       </c>
       <c r="G107" t="n">
-        <v>-7.83739</v>
-      </c>
-      <c r="H107" t="n">
         <v>110.174762</v>
       </c>
-      <c r="I107" t="b">
-        <v>0</v>
+      <c r="H107" t="b">
+        <v>0</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Barokah/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afae55a95524f:0x55116c0c1ee10332!8m2!3d-7.83739!4d110.1747618!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBXN0b3JlmgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVU5pYjNSMmJUbEJSUkFC4AEA-gEECAAQQA!16s%2Fg%2F11gdknz4jd?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J107" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Barokah/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afae55a95524f:0x55116c0c1ee10332!8m2!3d-7.83739!4d110.1747618!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBBXN0b3JlmgEkQ2hkRFNVaE5NRzluUzBWSlEwRm5TVU5pYjNSMmJUbEJSUkFC4AEA-gEECAAQQA!16s%2Fg%2F11gdknz4jd?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K107" t="inlineStr">
         <is>
           <t>21 jam lalu</t>
         </is>
@@ -4709,25 +4598,24 @@
       </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr"/>
+      <c r="E108" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F108" t="n">
-        <v>4.8</v>
+        <v>-7.858694</v>
       </c>
       <c r="G108" t="n">
-        <v>-7.858694</v>
-      </c>
-      <c r="H108" t="n">
         <v>110.171476</v>
       </c>
-      <c r="I108" t="b">
-        <v>0</v>
+      <c r="H108" t="b">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Oleh-oleh+Tiga+Jempol/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb55e1139407:0x7c21d941e5407a25!8m2!3d-7.8586939!4d110.1714761!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDWdyb2Nlcnlfc3RvcmWaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVUkdkRm8zVDFkM0VBReABAPoBBAgAEC0!16s%2Fg%2F11vhz7_b7r?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J108" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Oleh-oleh+Tiga+Jempol/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb55e1139407:0x7c21d941e5407a25!8m2!3d-7.8586939!4d110.1714761!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDWdyb2Nlcnlfc3RvcmWaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVUkdkRm8zVDFkM0VBReABAPoBBAgAEC0!16s%2Fg%2F11vhz7_b7r?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K108" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -4750,25 +4638,24 @@
           <t>0819-1707-2170</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr"/>
+      <c r="E109" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F109" t="n">
-        <v>4.6</v>
+        <v>-7.886461</v>
       </c>
       <c r="G109" t="n">
-        <v>-7.886461</v>
-      </c>
-      <c r="H109" t="n">
         <v>110.05822</v>
       </c>
-      <c r="I109" t="b">
-        <v>0</v>
+      <c r="H109" t="b">
+        <v>0</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/J%26C+Pusat+Oleh+Oleh+Khas+Jogja/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae51eece244a7:0x4f6b9be163cfa81c!8m2!3d-7.8864615!4d110.0582195!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBD3Nob3BwaW5nX2NlbnRlcuABAA!16s%2Fg%2F11lkx2qk5q?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J109" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/J%26C+Pusat+Oleh+Oleh+Khas+Jogja/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7ae51eece244a7:0x4f6b9be163cfa81c!8m2!3d-7.8864615!4d110.0582195!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBD3Nob3BwaW5nX2NlbnRlcuABAA!16s%2Fg%2F11lkx2qk5q?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K109" t="inlineStr">
         <is>
           <t>3 minggu lalu</t>
         </is>
@@ -4791,25 +4678,24 @@
           <t>0815-7989-746</t>
         </is>
       </c>
-      <c r="E110" t="inlineStr"/>
+      <c r="E110" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F110" t="n">
-        <v>4.6</v>
+        <v>-7.851292</v>
       </c>
       <c r="G110" t="n">
-        <v>-7.851292</v>
-      </c>
-      <c r="H110" t="n">
         <v>110.158786</v>
       </c>
-      <c r="I110" t="b">
-        <v>0</v>
+      <c r="H110" t="b">
+        <v>0</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bakpia+Pathuk+Rahmat/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb2137dedef1:0x75ed77daab1ec6ee!8m2!3d-7.8512923!4d110.1587856!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDWZvb2RfcHJvZHVjZXKaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVTnFaMUJZUkhoQlJSQULgAQD6AQQIABA9!16s%2Fg%2F11c7sbvplz?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J110" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Bakpia+Pathuk+Rahmat/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb2137dedef1:0x75ed77daab1ec6ee!8m2!3d-7.8512923!4d110.1587856!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBDWZvb2RfcHJvZHVjZXKaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVTnFaMUJZUkhoQlJSQULgAQD6AQQIABA9!16s%2Fg%2F11c7sbvplz?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K110" t="inlineStr">
         <is>
           <t>3 hari lalu</t>
         </is>
@@ -4832,25 +4718,24 @@
           <t>0851-0061-6764</t>
         </is>
       </c>
-      <c r="E111" t="inlineStr"/>
+      <c r="E111" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F111" t="n">
-        <v>4.3</v>
+        <v>-7.859594</v>
       </c>
       <c r="G111" t="n">
-        <v>-7.859594</v>
-      </c>
-      <c r="H111" t="n">
         <v>110.158656</v>
       </c>
-      <c r="I111" t="b">
-        <v>0</v>
+      <c r="H111" t="b">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Oleh+Oleh+Bu+Emi/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb3c9bbcdf47:0xeee3c731f8d7a4d4!8m2!3d-7.8595943!4d110.1586562!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb5IBD3Nob3BwaW5nX2NlbnRlcuABAA!16s%2Fg%2F11d_cxkzt0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J111" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Oleh+Oleh+Bu+Emi/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb3c9bbcdf47:0xeee3c731f8d7a4d4!8m2!3d-7.8595943!4d110.1586562!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb5IBD3Nob3BwaW5nX2NlbnRlcuABAA!16s%2Fg%2F11d_cxkzt0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K111" t="inlineStr">
         <is>
           <t>5 tahun lalu</t>
         </is>
@@ -4873,25 +4758,24 @@
           <t>0851-0061-6764</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr"/>
+      <c r="E112" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F112" t="n">
-        <v>4.3</v>
+        <v>-7.859594</v>
       </c>
       <c r="G112" t="n">
-        <v>-7.859594</v>
-      </c>
-      <c r="H112" t="n">
         <v>110.158656</v>
       </c>
-      <c r="I112" t="b">
-        <v>0</v>
+      <c r="H112" t="b">
+        <v>0</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Oleh+Oleh+Bu+Emi/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb3c9bbcdf47:0xeee3c731f8d7a4d4!8m2!3d-7.8595943!4d110.1586562!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb5IBD3Nob3BwaW5nX2NlbnRlcuABAA!16s%2Fg%2F11d_cxkzt0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J112" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Oleh+Oleh+Bu+Emi/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afb3c9bbcdf47:0xeee3c731f8d7a4d4!8m2!3d-7.8595943!4d110.1586562!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb5IBD3Nob3BwaW5nX2NlbnRlcuABAA!16s%2Fg%2F11d_cxkzt0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K112" t="inlineStr">
         <is>
           <t>5 tahun lalu</t>
         </is>
@@ -4918,25 +4802,24 @@
           <t>0813-6244-4414</t>
         </is>
       </c>
-      <c r="E113" t="inlineStr"/>
+      <c r="E113" t="n">
+        <v>5</v>
+      </c>
       <c r="F113" t="n">
-        <v>5</v>
+        <v>-7.866406</v>
       </c>
       <c r="G113" t="n">
-        <v>-7.866406</v>
-      </c>
-      <c r="H113" t="n">
         <v>110.160152</v>
       </c>
-      <c r="I113" t="b">
-        <v>0</v>
+      <c r="H113" t="b">
+        <v>0</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Aki+Shop+Kulon+Progo+24jam/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afbe6a6da70e3:0x322ccc4fd46007d4!8m2!3d-7.8664056!4d110.1601524!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBEWNhcl9iYXR0ZXJ5X3N0b3Jl4AEA!16s%2Fg%2F11l6bg84_8?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J113" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Aki+Shop+Kulon+Progo+24jam/@-7.865617,109.870864,11z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Kulon+Progo!6e6!3m6!1s0x2e7afbe6a6da70e3:0x322ccc4fd46007d4!8m2!3d-7.8664056!4d110.1601524!15sChpUb2tvIE9sZWggb2xlaCBLdWxvbiBQcm9nb1ocIhp0b2tvIG9sZWggb2xlaCBrdWxvbiBwcm9nb5IBEWNhcl9iYXR0ZXJ5X3N0b3Jl4AEA!16s%2Fg%2F11l6bg84_8?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K113" t="inlineStr">
         <is>
           <t>1 hari lalu</t>
         </is>
@@ -4954,16 +4837,15 @@
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
-      <c r="H114" t="inlineStr"/>
-      <c r="I114" t="b">
-        <v>0</v>
-      </c>
-      <c r="J114" t="inlineStr">
+      <c r="H114" t="b">
+        <v>0</v>
+      </c>
+      <c r="I114" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/search/Toko+Oleh+oleh+Sleman/@-7.8053374,110.3684985,15z/data=!4m2!2m1!6e6?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4986,25 +4868,24 @@
           <t>(0274) 489898</t>
         </is>
       </c>
-      <c r="E115" t="inlineStr"/>
+      <c r="E115" t="n">
+        <v>4.1</v>
+      </c>
       <c r="F115" t="n">
-        <v>4.1</v>
+        <v>-7.783273</v>
       </c>
       <c r="G115" t="n">
-        <v>-7.783273</v>
-      </c>
-      <c r="H115" t="n">
         <v>110.428878</v>
       </c>
-      <c r="I115" t="b">
-        <v>0</v>
+      <c r="H115" t="b">
+        <v>0</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pusat+oleh-oleh+DJOE/@-7.7832729,110.4108539,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5a02d9d2e3df:0xe05944fd425b98ca!8m2!3d-7.7832729!4d110.4288783!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F11c1wwylfx?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J115" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pusat+oleh-oleh+DJOE/@-7.7832729,110.4108539,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5a02d9d2e3df:0xe05944fd425b98ca!8m2!3d-7.7832729!4d110.4288783!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEOc291dmVuaXJfc3RvcmXgAQA!16s%2Fg%2F11c1wwylfx?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K115" t="inlineStr">
         <is>
           <t>2 minggu lalu</t>
         </is>
@@ -5027,25 +4908,24 @@
           <t>0818-0432-0927</t>
         </is>
       </c>
-      <c r="E116" t="inlineStr"/>
+      <c r="E116" t="n">
+        <v>5</v>
+      </c>
       <c r="F116" t="n">
-        <v>5</v>
+        <v>-7.66901</v>
       </c>
       <c r="G116" t="n">
-        <v>-7.66901</v>
-      </c>
-      <c r="H116" t="n">
         <v>110.333076</v>
       </c>
-      <c r="I116" t="b">
-        <v>0</v>
+      <c r="H116" t="b">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Oleh+oleh+khas+Jogja/@-7.6690097,110.3150518,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5f27fc4c38a5:0x68c6566363ad22a5!8m2!3d-7.6690097!4d110.3330762!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEFc3RvcmXgAQA!16s%2Fg%2F11pvf9p_nj?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J116" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Oleh+oleh+khas+Jogja/@-7.6690097,110.3150518,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5f27fc4c38a5:0x68c6566363ad22a5!8m2!3d-7.6690097!4d110.3330762!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEFc3RvcmXgAQA!16s%2Fg%2F11pvf9p_nj?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K116" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -5064,25 +4944,24 @@
       </c>
       <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr"/>
-      <c r="E117" t="inlineStr"/>
+      <c r="E117" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F117" t="n">
-        <v>4.5</v>
+        <v>-7.660604</v>
       </c>
       <c r="G117" t="n">
-        <v>-7.660604</v>
-      </c>
-      <c r="H117" t="n">
         <v>110.371231</v>
       </c>
-      <c r="I117" t="b">
-        <v>0</v>
+      <c r="H117" t="b">
+        <v>0</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Oleh-Oleh+Sleman+(Aneka+Olahan+Salak+Cristal)/@-7.6606038,110.3532063,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5fb195b5eefd:0xa740fe9cf1ee84e6!8m2!3d-7.6606038!4d110.3712307!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgENZ3JlZW5fZ3JvY2Vyc-ABAA!16s%2Fg%2F11bx8hkkyw?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J117" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Oleh-Oleh+Sleman+(Aneka+Olahan+Salak+Cristal)/@-7.6606038,110.3532063,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5fb195b5eefd:0xa740fe9cf1ee84e6!8m2!3d-7.6606038!4d110.3712307!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgENZ3JlZW5fZ3JvY2Vyc-ABAA!16s%2Fg%2F11bx8hkkyw?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K117" t="inlineStr">
         <is>
           <t>7 bulan lalu</t>
         </is>
@@ -5105,25 +4984,24 @@
           <t>0822-2555-7758</t>
         </is>
       </c>
-      <c r="E118" t="inlineStr"/>
+      <c r="E118" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F118" t="n">
-        <v>4.5</v>
+        <v>-7.719986</v>
       </c>
       <c r="G118" t="n">
-        <v>-7.719986</v>
-      </c>
-      <c r="H118" t="n">
         <v>110.403584</v>
       </c>
-      <c r="I118" t="b">
-        <v>0</v>
-      </c>
-      <c r="J118" t="inlineStr">
+      <c r="H118" t="b">
+        <v>0</v>
+      </c>
+      <c r="I118" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Toko+Oleh-Oleh+Bakpia+Pathok+Rizky+Pusat+(Gentan)/@-7.7199862,110.3855592,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5914f142a1c3:0x6b12e38fa1d71644!8m2!3d-7.7199862!4d110.4035836!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEEZGVsaeABAA!16s%2Fg%2F11h1zw2cq0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5142,25 +5020,24 @@
           <t>(0274) 562985</t>
         </is>
       </c>
-      <c r="E119" t="inlineStr"/>
+      <c r="E119" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F119" t="n">
-        <v>4.5</v>
+        <v>-7.75836</v>
       </c>
       <c r="G119" t="n">
-        <v>-7.75836</v>
-      </c>
-      <c r="H119" t="n">
         <v>110.400102</v>
       </c>
-      <c r="I119" t="b">
-        <v>0</v>
+      <c r="H119" t="b">
+        <v>0</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bakpia+Mutiara+Jogja+-+Ruko+Depan+Polda+Sleman/@-7.7583603,110.3820774,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a59a4e3ff6a37:0x94c10ede1fd5b886!8m2!3d-7.7583603!4d110.4001018!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11pwvff2yw?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J119" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Bakpia+Mutiara+Jogja+-+Ruko+Depan+Polda+Sleman/@-7.7583603,110.3820774,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a59a4e3ff6a37:0x94c10ede1fd5b886!8m2!3d-7.7583603!4d110.4001018!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11pwvff2yw?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K119" t="inlineStr">
         <is>
           <t>3 minggu lalu</t>
         </is>
@@ -5187,25 +5064,24 @@
           <t>0878-7878-0251</t>
         </is>
       </c>
-      <c r="E120" t="inlineStr"/>
+      <c r="E120" t="n">
+        <v>5</v>
+      </c>
       <c r="F120" t="n">
-        <v>5</v>
+        <v>-7.783388</v>
       </c>
       <c r="G120" t="n">
-        <v>-7.783388</v>
-      </c>
-      <c r="H120" t="n">
         <v>110.401157</v>
       </c>
-      <c r="I120" t="b">
-        <v>0</v>
+      <c r="H120" t="b">
+        <v>0</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Oleh-Oleh+Jogja+Amplaz+Malio17/@-7.7833879,110.3831324,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a573b437d1a03:0xbd1eb7212935c781!8m2!3d-7.7833879!4d110.4011568!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEFc3RvcmXgAQA!16s%2Fg%2F11k9cyyx19?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J120" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Oleh-Oleh+Jogja+Amplaz+Malio17/@-7.7833879,110.3831324,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a573b437d1a03:0xbd1eb7212935c781!8m2!3d-7.7833879!4d110.4011568!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEFc3RvcmXgAQA!16s%2Fg%2F11k9cyyx19?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K120" t="inlineStr">
         <is>
           <t>2 bulan lalu</t>
         </is>
@@ -5228,25 +5104,24 @@
           <t>(0274) 866129</t>
         </is>
       </c>
-      <c r="E121" t="inlineStr"/>
+      <c r="E121" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F121" t="n">
-        <v>4.4</v>
+        <v>-7.695</v>
       </c>
       <c r="G121" t="n">
-        <v>-7.695</v>
-      </c>
-      <c r="H121" t="n">
         <v>110.34563</v>
       </c>
-      <c r="I121" t="b">
-        <v>0</v>
-      </c>
-      <c r="J121" t="inlineStr">
+      <c r="H121" t="b">
+        <v>0</v>
+      </c>
+      <c r="I121" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/PUSAT+OLEH+-+OLEH+MANGGA+TIGA/@-7.6950002,110.3276058,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5f428896bbab:0xdfed257f767baedc!8m2!3d-7.6950002!4d110.3456302!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEFc3RvcmWaASRDaGREU1VoTk1HOW5TMFZKUTBGblNVTnVNVkJQWWpkUlJSQULgAQD6AQQIABA0!16s%2Fg%2F11c56s8__7?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5269,25 +5144,24 @@
           <t>0895-3286-67027</t>
         </is>
       </c>
-      <c r="E122" t="inlineStr"/>
+      <c r="E122" t="n">
+        <v>4.3</v>
+      </c>
       <c r="F122" t="n">
-        <v>4.3</v>
+        <v>-7.746364</v>
       </c>
       <c r="G122" t="n">
-        <v>-7.746364</v>
-      </c>
-      <c r="H122" t="n">
         <v>110.405952</v>
       </c>
-      <c r="I122" t="b">
-        <v>0</v>
+      <c r="H122" t="b">
+        <v>0</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bakpia+Mino+805/@-7.7463638,110.3879273,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5973b3b50eeb:0xee2733e39d2f7f80!8m2!3d-7.7463638!4d110.4059517!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEJY2FrZV9zaG9w4AEA!16s%2Fg%2F11bxg5yp6k?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J122" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Bakpia+Mino+805/@-7.7463638,110.3879273,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5973b3b50eeb:0xee2733e39d2f7f80!8m2!3d-7.7463638!4d110.4059517!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEJY2FrZV9zaG9w4AEA!16s%2Fg%2F11bxg5yp6k?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K122" t="inlineStr">
         <is>
           <t>4 minggu lalu</t>
         </is>
@@ -5310,25 +5184,24 @@
           <t>0852-9202-2822</t>
         </is>
       </c>
-      <c r="E123" t="inlineStr"/>
+      <c r="E123" t="n">
+        <v>3.7</v>
+      </c>
       <c r="F123" t="n">
-        <v>3.7</v>
+        <v>-7.753016</v>
       </c>
       <c r="G123" t="n">
-        <v>-7.753016</v>
-      </c>
-      <c r="H123" t="n">
         <v>110.393121</v>
       </c>
-      <c r="I123" t="b">
-        <v>0</v>
+      <c r="H123" t="b">
+        <v>0</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Buku+Jogjakarta+Sleman/@-7.7530162,110.3750962,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a59cb68c65a7d:0x69dd22b694d3d92b!8m2!3d-7.7530162!4d110.3931206!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW6SAQpib29rX3N0b3Jl4AEA!16s%2Fg%2F11hdng_w06?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J123" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Buku+Jogjakarta+Sleman/@-7.7530162,110.3750962,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a59cb68c65a7d:0x69dd22b694d3d92b!8m2!3d-7.7530162!4d110.3931206!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW6SAQpib29rX3N0b3Jl4AEA!16s%2Fg%2F11hdng_w06?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K123" t="inlineStr">
         <is>
           <t>4 bulan lalu</t>
         </is>
@@ -5355,25 +5228,24 @@
           <t>(0274) 566122</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr"/>
+      <c r="E124" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F124" t="n">
-        <v>4.6</v>
+        <v>-7.796894</v>
       </c>
       <c r="G124" t="n">
-        <v>-7.796894</v>
-      </c>
-      <c r="H124" t="n">
         <v>110.357974</v>
       </c>
-      <c r="I124" t="b">
-        <v>0</v>
+      <c r="H124" t="b">
+        <v>0</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pabrik+Bakpia+Pathok+25/@-7.7968937,110.3399494,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a578e196cf7c9:0xa47522a4f2b4fcdc!8m2!3d-7.7968937!4d110.3579738!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEZZm9vZF9tYW51ZmFjdHVyaW5nX3N1cHBseeABAA!16s%2Fg%2F1hm29l42j?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J124" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Pabrik+Bakpia+Pathok+25/@-7.7968937,110.3399494,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a578e196cf7c9:0xa47522a4f2b4fcdc!8m2!3d-7.7968937!4d110.3579738!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEZZm9vZF9tYW51ZmFjdHVyaW5nX3N1cHBseeABAA!16s%2Fg%2F1hm29l42j?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K124" t="inlineStr">
         <is>
           <t>21 jam lalu</t>
         </is>
@@ -5396,25 +5268,24 @@
           <t>(0274) 4463151</t>
         </is>
       </c>
-      <c r="E125" t="inlineStr"/>
+      <c r="E125" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F125" t="n">
-        <v>4.5</v>
+        <v>-7.752631</v>
       </c>
       <c r="G125" t="n">
-        <v>-7.752631</v>
-      </c>
-      <c r="H125" t="n">
         <v>110.398499</v>
       </c>
-      <c r="I125" t="b">
-        <v>0</v>
+      <c r="H125" t="b">
+        <v>0</v>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Merah+Condongcatur/@-7.7526315,110.3804742,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a590bbb7fd797:0xe43caaaccc7d7144!8m2!3d-7.7526315!4d110.3984986!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEQc3RhdGlvbmVyeV9zdG9yZZoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VSaGRFb3RUMlZCRUFF4AEA-gEECAAQSQ!16s%2Fg%2F1pt_4f678?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J125" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Merah+Condongcatur/@-7.7526315,110.3804742,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a590bbb7fd797:0xe43caaaccc7d7144!8m2!3d-7.7526315!4d110.3984986!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEQc3RhdGlvbmVyeV9zdG9yZZoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VSaGRFb3RUMlZCRUFF4AEA-gEECAAQSQ!16s%2Fg%2F1pt_4f678?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K125" t="inlineStr">
         <is>
           <t>3 hari lalu</t>
         </is>
@@ -5433,25 +5304,24 @@
       </c>
       <c r="C126" t="inlineStr"/>
       <c r="D126" t="inlineStr"/>
-      <c r="E126" t="inlineStr"/>
+      <c r="E126" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F126" t="n">
-        <v>4.5</v>
+        <v>-7.741758</v>
       </c>
       <c r="G126" t="n">
-        <v>-7.741758</v>
-      </c>
-      <c r="H126" t="n">
         <v>110.408037</v>
       </c>
-      <c r="I126" t="b">
-        <v>0</v>
+      <c r="H126" t="b">
+        <v>0</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Flamboyan/@-7.7417579,110.3900123,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a59723de85659:0xd8aa3924bcb6a078!8m2!3d-7.7417579!4d110.4080367!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgELc3VwZXJtYXJrZXSaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVUkVOamcyUzFsUkVBReABAPoBBAhJEEI!16s%2Fg%2F11csc7w9nd?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J126" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Flamboyan/@-7.7417579,110.3900123,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a59723de85659:0xd8aa3924bcb6a078!8m2!3d-7.7417579!4d110.4080367!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgELc3VwZXJtYXJrZXSaASNDaFpEU1VoTk1HOW5TMFZKUTBGblNVUkVOamcyUzFsUkVBReABAPoBBAhJEEI!16s%2Fg%2F11csc7w9nd?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K126" t="inlineStr">
         <is>
           <t>4 bulan lalu</t>
         </is>
@@ -5474,25 +5344,24 @@
           <t>0857-2960-4331</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr"/>
+      <c r="E127" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F127" t="n">
-        <v>4.6</v>
+        <v>-7.74455</v>
       </c>
       <c r="G127" t="n">
-        <v>-7.74455</v>
-      </c>
-      <c r="H127" t="n">
         <v>110.389487</v>
       </c>
-      <c r="I127" t="b">
-        <v>0</v>
+      <c r="H127" t="b">
+        <v>0</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Toko+Keramik+pecah+belah/@-7.74455,110.3714623,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a590543ba221d:0xcc8e52a3d5146706!8m2!3d-7.74455!4d110.3894867!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEQaG9tZV9nb29kc19zdG9yZZoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VOTGJVeDJZMmRSUlJBQuABAPoBBAgAED4!16s%2Fg%2F11c37_y46j?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J127" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Toko+Keramik+pecah+belah/@-7.74455,110.3714623,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a590543ba221d:0xcc8e52a3d5146706!8m2!3d-7.74455!4d110.3894867!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEQaG9tZV9nb29kc19zdG9yZZoBJENoZERTVWhOTUc5blMwVkpRMEZuU1VOTGJVeDJZMmRSUlJBQuABAPoBBAgAED4!16s%2Fg%2F11c37_y46j?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K127" t="inlineStr">
         <is>
           <t>sebulan lalu</t>
         </is>
@@ -5519,25 +5388,24 @@
           <t>0856-0097-0799</t>
         </is>
       </c>
-      <c r="E128" t="inlineStr"/>
+      <c r="E128" t="n">
+        <v>4.4</v>
+      </c>
       <c r="F128" t="n">
-        <v>4.4</v>
+        <v>-7.746481</v>
       </c>
       <c r="G128" t="n">
-        <v>-7.746481</v>
-      </c>
-      <c r="H128" t="n">
         <v>110.412244</v>
       </c>
-      <c r="I128" t="b">
-        <v>0</v>
+      <c r="H128" t="b">
+        <v>0</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Berly+Bread+Jambusari/@-7.7464811,110.3942191,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a595ffa0e3487:0xedcde2c3c3d164a5!8m2!3d-7.7464811!4d110.4122435!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11j2ccw4tb?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J128" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Berly+Bread+Jambusari/@-7.7464811,110.3942191,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a595ffa0e3487:0xedcde2c3c3d164a5!8m2!3d-7.7464811!4d110.4122435!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11j2ccw4tb?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K128" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -5564,25 +5432,24 @@
           <t>0878-3991-6613</t>
         </is>
       </c>
-      <c r="E129" t="inlineStr"/>
+      <c r="E129" t="n">
+        <v>4.9</v>
+      </c>
       <c r="F129" t="n">
-        <v>4.9</v>
+        <v>-7.745393</v>
       </c>
       <c r="G129" t="n">
-        <v>-7.745393</v>
-      </c>
-      <c r="H129" t="n">
         <v>110.398177</v>
       </c>
-      <c r="I129" t="b">
-        <v>0</v>
+      <c r="H129" t="b">
+        <v>0</v>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Artlinx+Store/@-7.7453926,110.380153,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a59a7e6b66fd5:0x98dfdf689fa1241c!8m2!3d-7.7453926!4d110.3981774!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEQc3RhdGlvbmVyeV9zdG9yZeABAA!16s%2Fg%2F11g6hwlhw5?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J129" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Artlinx+Store/@-7.7453926,110.380153,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a59a7e6b66fd5:0x98dfdf689fa1241c!8m2!3d-7.7453926!4d110.3981774!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEQc3RhdGlvbmVyeV9zdG9yZeABAA!16s%2Fg%2F11g6hwlhw5?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K129" t="inlineStr">
         <is>
           <t>23 jam lalu</t>
         </is>
@@ -5605,25 +5472,24 @@
           <t>0857-2590-7688</t>
         </is>
       </c>
-      <c r="E130" t="inlineStr"/>
+      <c r="E130" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F130" t="n">
-        <v>4.5</v>
+        <v>-7.743472</v>
       </c>
       <c r="G130" t="n">
-        <v>-7.743472</v>
-      </c>
-      <c r="H130" t="n">
         <v>110.389751</v>
       </c>
-      <c r="I130" t="b">
-        <v>0</v>
+      <c r="H130" t="b">
+        <v>0</v>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/ChezMoi+Patissier+%26+Chocolatier+Jl.+Kaliurang/@-7.7434719,110.3717262,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a590552a8e3e9:0x35e362a356b259ab!8m2!3d-7.7434719!4d110.3897506!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11b61rbdrq?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J130" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/ChezMoi+Patissier+%26+Chocolatier+Jl.+Kaliurang/@-7.7434719,110.3717262,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a590552a8e3e9:0x35e362a356b259ab!8m2!3d-7.7434719!4d110.3897506!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11b61rbdrq?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K130" t="inlineStr">
         <is>
           <t>2 minggu lalu</t>
         </is>
@@ -5646,25 +5512,24 @@
           <t>0813-2532-6932</t>
         </is>
       </c>
-      <c r="E131" t="inlineStr"/>
+      <c r="E131" t="n">
+        <v>4.8</v>
+      </c>
       <c r="F131" t="n">
-        <v>4.8</v>
+        <v>-7.73654</v>
       </c>
       <c r="G131" t="n">
-        <v>-7.73654</v>
-      </c>
-      <c r="H131" t="n">
         <v>110.39419</v>
       </c>
-      <c r="I131" t="b">
-        <v>0</v>
+      <c r="H131" t="b">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/AIS+AKI+Sleman/@-7.7434719,110.3717262,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5916e899564d:0xac115e40f200be3f!8m2!3d-7.7365405!4d110.3941899!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgERY2FyX2JhdHRlcnlfc3RvcmXgAQA!16s%2Fg%2F11bw61ghrz?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J131" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/AIS+AKI+Sleman/@-7.7434719,110.3717262,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5916e899564d:0xac115e40f200be3f!8m2!3d-7.7365405!4d110.3941899!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgERY2FyX2JhdHRlcnlfc3RvcmXgAQA!16s%2Fg%2F11bw61ghrz?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K131" t="inlineStr">
         <is>
           <t>seminggu lalu</t>
         </is>
@@ -5687,25 +5552,24 @@
           <t>0896-8698-7227</t>
         </is>
       </c>
-      <c r="E132" t="inlineStr"/>
+      <c r="E132" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F132" t="n">
-        <v>4.5</v>
+        <v>-7.718937</v>
       </c>
       <c r="G132" t="n">
-        <v>-7.718937</v>
-      </c>
-      <c r="H132" t="n">
         <v>110.404961</v>
       </c>
-      <c r="I132" t="b">
-        <v>0</v>
-      </c>
-      <c r="J132" t="inlineStr">
+      <c r="H132" t="b">
+        <v>0</v>
+      </c>
+      <c r="I132" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Ollin+Bakery+%26+Cakeshop/@-7.7189375,110.386937,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a5949af2e5b83:0x1aae8f5c6a5a7b3d!8m2!3d-7.7189375!4d110.4049614!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11b6smfd56?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K132" t="inlineStr"/>
+      <c r="J132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5724,25 +5588,24 @@
           <t>0896-8698-7227</t>
         </is>
       </c>
-      <c r="E133" t="inlineStr"/>
+      <c r="E133" t="n">
+        <v>4.5</v>
+      </c>
       <c r="F133" t="n">
-        <v>4.5</v>
+        <v>-7.74568</v>
       </c>
       <c r="G133" t="n">
-        <v>-7.74568</v>
-      </c>
-      <c r="H133" t="n">
         <v>110.406686</v>
       </c>
-      <c r="I133" t="b">
-        <v>0</v>
+      <c r="H133" t="b">
+        <v>0</v>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Wisli+Bakery/@-7.7456799,110.388662,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a599f42ec3e33:0x9618c02be5631719!8m2!3d-7.7456799!4d110.4066864!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11qhw6qdx0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
+        </is>
       </c>
       <c r="J133" t="inlineStr">
-        <is>
-          <t>https://www.google.com/maps/place/Wisli+Bakery/@-7.7456799,110.388662,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a599f42ec3e33:0x9618c02be5631719!8m2!3d-7.7456799!4d110.4066864!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11qhw6qdx0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
-        </is>
-      </c>
-      <c r="K133" t="inlineStr">
         <is>
           <t>setahun lalu</t>
         </is>
@@ -5765,25 +5628,24 @@
           <t>0877-4400-5757</t>
         </is>
       </c>
-      <c r="E134" t="inlineStr"/>
+      <c r="E134" t="n">
+        <v>4.6</v>
+      </c>
       <c r="F134" t="n">
-        <v>4.6</v>
+        <v>-7.74568</v>
       </c>
       <c r="G134" t="n">
-        <v>-7.74568</v>
-      </c>
-      <c r="H134" t="n">
         <v>110.406686</v>
       </c>
-      <c r="I134" t="b">
-        <v>0</v>
-      </c>
-      <c r="J134" t="inlineStr">
+      <c r="H134" t="b">
+        <v>0</v>
+      </c>
+      <c r="I134" t="inlineStr">
         <is>
           <t>https://www.google.com/maps/place/Wisli+Bakery/@-7.7456799,110.388662,15z/data=!4m11!1m3!2m2!1sToko+Oleh+oleh+Sleman!6e6!3m6!1s0x2e7a599f42ec3e33:0x9618c02be5631719!8m2!3d-7.7456799!4d110.4066864!15sChVUb2tvIE9sZWggb2xlaCBTbGVtYW5aFyIVdG9rbyBvbGVoIG9sZWggc2xlbWFukgEGYmFrZXJ54AEA!16s%2Fg%2F11qhw6qdx0?entry=ttu&amp;g_ep=EgoyMDI1MDIwMi4wIKXMDSoASAFQAw%3D%3D</t>
         </is>
       </c>
-      <c r="K134" t="inlineStr"/>
+      <c r="J134" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>